<commit_message>
Serie Bob Construye, construcciones ecológicas SD y HD 101
</commit_message>
<xml_diff>
--- a/Run_File.xlsx
+++ b/Run_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0059819-8CE7-4E00-8C16-8246A6DC35BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5E62C3-359B-428A-94ED-0C9AF06F1803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
   </bookViews>
   <sheets>
     <sheet name="SD" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="89">
   <si>
     <t>Creation_Date</t>
   </si>
@@ -233,427 +233,76 @@
     <t>FileName</t>
   </si>
   <si>
-    <t>TV-Y</t>
+    <t>EEBOBG101_SD_ADI.XML</t>
   </si>
   <si>
-    <t>EP 02</t>
+    <t>EEBO6000000000000101</t>
   </si>
   <si>
-    <t>EP 03</t>
+    <t>Serie Bob Construye, construcciones ecológicas</t>
   </si>
   <si>
-    <t>EP 04</t>
+    <t>Bob Construye, construcciones ecológicasT01EP01</t>
   </si>
   <si>
-    <t>EP 05</t>
+    <t>Bob Construye, construcciones ecológicas T01 EP01</t>
   </si>
   <si>
-    <t>EP 06</t>
+    <t>Edye presenta: Bob está de vuelta en el sitio. Únete a Bob mientras te muestra el increíble mundo de hogares ecológicos y centros de reciclaje.</t>
   </si>
   <si>
-    <t>EP 07</t>
+    <t>Edye presenta: Bob está de vuelta en el sitio. Únase a Bob mientras le muestra el asombroso mundo de las casas ecológicas y los centros de reciclaje y aprenda cómo las cosas que tira pueden usarse para hacer algo nuevo. Vea cómo todos pueden unirse y divertirse construyendo casas ecológicas.</t>
   </si>
   <si>
-    <t>EP 08</t>
+    <t>G</t>
   </si>
   <si>
-    <t>EP 09</t>
+    <t>01:00:05</t>
   </si>
   <si>
-    <t>EP 10</t>
+    <t>01:00</t>
   </si>
   <si>
-    <t>EEANME201_SD_ADI.XML</t>
+    <t>Infantil/Bob Construye, construcciones ecológicas</t>
   </si>
   <si>
-    <t>EEAN6000000000000201</t>
+    <t>Bob Construye, construcciones ecológicas</t>
   </si>
   <si>
-    <t>Serie Mecanimales</t>
+    <t>UK</t>
   </si>
   <si>
-    <t>MecanimalesT02EP01</t>
+    <t>Neil Morrissey</t>
   </si>
   <si>
-    <t>Mecanimales T02 EP01</t>
+    <t>HIT Ent. Ltd Keith</t>
   </si>
   <si>
-    <t>Edye presenta: La misión de los Mecanimales es lograr que la Mecanimontaña Rusa funcione de nuevo.</t>
+    <t>Morrissey Neil</t>
   </si>
   <si>
-    <t>Edye presenta: La misión de los Mecanimales es lograr que la Mecanimontaña Rusa funcione de nuevo. Llegan a la Isla de la Mecanimontaña Rusa y descubren que el problema es un Mecanimono que cuelga de los rieles del tren.</t>
+    <t>Little, Brian</t>
   </si>
   <si>
-    <t>00:11:30</t>
+    <t>EEBOBG101.mpg</t>
   </si>
   <si>
-    <t>00:11</t>
+    <t>EEBOBG1_box.jpg</t>
   </si>
   <si>
-    <t>Infantil/Mecanimales</t>
+    <t>EEBOBG101_land.jpg</t>
   </si>
   <si>
-    <t>Mecanimales</t>
+    <t>EEBOBG101_HD_ADI.XML</t>
   </si>
   <si>
-    <t>CA</t>
+    <t>EEBO7000000000000101</t>
   </si>
   <si>
-    <t>Gilly Fogg, Jim Fowler, Jess Rosen</t>
+    <t>Bob Construye, construcciones ecológicas T01 EP01 HD</t>
   </si>
   <si>
-    <t>Snap Prod. Inc.</t>
-  </si>
-  <si>
-    <t>Fogg Gilly, Fowler Jim, Rosen Jess</t>
-  </si>
-  <si>
-    <t>Fogg, Gilly</t>
-  </si>
-  <si>
-    <t>EEANME201.mpg</t>
-  </si>
-  <si>
-    <t>EEANME2_box.jpg</t>
-  </si>
-  <si>
-    <t>EEANME201_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME202_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000202</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP02</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP02</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los tímidos Mecanipandas necesitan ayuda para alcanzar sus bocadillos favoritos de bambú.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los tímidos Mecanipandas necesitan ayuda para alcanzar sus bocadillos favoritos de bambú en la cima de una montaña resbaladiza. Mientras el fuerte Rex empuja los Pandas cuesta arriba, Unicornio vuela y arrastra a los demás Mecanimales.</t>
-  </si>
-  <si>
-    <t>EEANME202.mpg</t>
-  </si>
-  <si>
-    <t>EEANME202_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME203_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000203</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP03</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP03</t>
-  </si>
-  <si>
-    <t>Edye presenta: El Mecanicucú dejó de funcionar y los Mecanimales deberán descubrir por qué.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El Mecanicucú dejó de funcionar y la misión de los Mecanimales ahora es descubrir el por qué. Sin embargo, rápidamente hallan el problema: algunos de los números del reloj han desaparecido.</t>
-  </si>
-  <si>
-    <t>EEANME203.mpg</t>
-  </si>
-  <si>
-    <t>EEANME203_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME204_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000204</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP04</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP04</t>
-  </si>
-  <si>
-    <t>Edye presenta: El Mecanicastor dejó de reciclar, y los Mecanimales deberán averiguar por qué.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El Mecanicastor dejó de reciclar, y los Mecanimales deberán resolver el problema antes de que la Isla del Mecanireciclador se llene de basura. Y cuando Unicornio comienza a investigar, vuela en lo alto y descubre al castor.</t>
-  </si>
-  <si>
-    <t>EEANME204.mpg</t>
-  </si>
-  <si>
-    <t>EEANME204_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME205_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000205</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP05</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP05</t>
-  </si>
-  <si>
-    <t>Edye presenta: La agradable música de la Isla de los Mecaniosos fue reemplazada por desagradables sonidos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: La música de la Isla de los Mecaniosos fue reemplazada por desagradables sonidos, lo que ocasiona que los osos bailen de forma muy extraña. Entonces, Rex intenta construir una fortaleza a prueba de sonido pero no es lo suficientemente acústica.</t>
-  </si>
-  <si>
-    <t>EEANME205.mpg</t>
-  </si>
-  <si>
-    <t>EEANME205_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME206_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000206</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP06</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP06</t>
-  </si>
-  <si>
-    <t>Edye presenta: La máquina de nubes no se siente bien y las nubes rosadas que generalmente flotan en el aire estan en el suelo</t>
-  </si>
-  <si>
-    <t>Edye presenta: La máquina de nubes no se siente muy bien, y las nubes rosadas que generalmente flotan en el aire por encima de ella están sentadas en el suelo. El equipo descubre que algo está atascado dentro de la máquina de nubes</t>
-  </si>
-  <si>
-    <t>EEANME206.mpg</t>
-  </si>
-  <si>
-    <t>EEANME206_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME207_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000207</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP07</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP07</t>
-  </si>
-  <si>
-    <t>Edye presenta: El equipo es enviado a la Isla del Babuino, donde deben encontrar un acondicionador de pera.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El equipo es enviado a la Isla del Babuino, donde su misión es encontrar un acondicionador de pera para que el babuino coma. Entonces, Sasquatch se estira para alcanzar las peras. Desafortunadamente, las deja volar.</t>
-  </si>
-  <si>
-    <t>EEANME207.mpg</t>
-  </si>
-  <si>
-    <t>EEANME207_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME208_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000208</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP08</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP08</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Mecanimales aprenden sobre parejas cuando visitan la Isla del Mecanicombinador.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Mecanimales aprenden sobre pares y parejas cuando visitan la Isla del Mecanicombinador para ayudarlo. Aparentemente el Mecanicombinador está combinando cosas que no suelen ir juntas.</t>
-  </si>
-  <si>
-    <t>EEANME208.mpg</t>
-  </si>
-  <si>
-    <t>EEANME208_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME209_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000209</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP09</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP09</t>
-  </si>
-  <si>
-    <t>Edye presenta: La misión del equipo es visitar la Isla del Mecaniesquí y arreglar el trampolín de esquí.</t>
-  </si>
-  <si>
-    <t>Edye presenta: La misión del equipo será ir a la Isla del Mecaniesquí y arreglar el trampolín de esquí, así los habitantes pueden jugar de nuevo. Komodo une las piezas pero luego descubre que los números de puntaje están mal puestos.</t>
-  </si>
-  <si>
-    <t>EEANME209.mpg</t>
-  </si>
-  <si>
-    <t>EEANME209_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME210_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN6000000000000210</t>
-  </si>
-  <si>
-    <t>MecanimalesT02EP10</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP10</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Mecanimales llegan a la Isla de los Mecanibotes para lograr que el faro funcione de nuevo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Mecanimales llegan a la Isla de los Mecanibotes para lograr que el faro funcione de nuevo, así los mecanibotes podrán guiarse en la niebla. Entonces, Unicornio usa sus poderes para hacer un puente de hielo y el equipo llega a la isla del faro.</t>
-  </si>
-  <si>
-    <t>EEANME210.mpg</t>
-  </si>
-  <si>
-    <t>EEANME210_land.jpg</t>
-  </si>
-  <si>
-    <t>EEANME201_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000201</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP01 HD</t>
-  </si>
-  <si>
-    <t>EEANME201.ts</t>
-  </si>
-  <si>
-    <t>EEANME202_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000202</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP02 HD</t>
-  </si>
-  <si>
-    <t>EEANME202.ts</t>
-  </si>
-  <si>
-    <t>EEANME203_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000203</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP03 HD</t>
-  </si>
-  <si>
-    <t>EEANME203.ts</t>
-  </si>
-  <si>
-    <t>EEANME204_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000204</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP04 HD</t>
-  </si>
-  <si>
-    <t>EEANME204.ts</t>
-  </si>
-  <si>
-    <t>EEANME205_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000205</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP05 HD</t>
-  </si>
-  <si>
-    <t>EEANME205.ts</t>
-  </si>
-  <si>
-    <t>EEANME206_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000206</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP06 HD</t>
-  </si>
-  <si>
-    <t>EEANME206.ts</t>
-  </si>
-  <si>
-    <t>EEANME207_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000207</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP07 HD</t>
-  </si>
-  <si>
-    <t>EEANME207.ts</t>
-  </si>
-  <si>
-    <t>EEANME208_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000208</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP08 HD</t>
-  </si>
-  <si>
-    <t>EEANME208.ts</t>
-  </si>
-  <si>
-    <t>EEANME209_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000209</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP09 HD</t>
-  </si>
-  <si>
-    <t>EEANME209.ts</t>
-  </si>
-  <si>
-    <t>EEANME210_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEAN7000000000000210</t>
-  </si>
-  <si>
-    <t>Mecanimales T02 EP10 HD</t>
-  </si>
-  <si>
-    <t>EEANME210.ts</t>
+    <t>EEBOBG101.ts</t>
   </si>
 </sst>
 </file>
@@ -6962,7 +6611,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:BF58"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:BF58"/>
     </sheetView>
   </sheetViews>
@@ -7143,10 +6792,10 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3">
-        <v>44621</v>
+        <v>44628</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -7167,13 +6816,13 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -7183,31 +6832,31 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>49</v>
@@ -7216,7 +6865,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43565</v>
+        <v>43742</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -7228,28 +6877,28 @@
         <v>31028</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AH2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AL2" s="6"/>
       <c r="AM2" s="6" t="s">
@@ -7271,7 +6920,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="6">
-        <v>324118204</v>
+        <v>1690768412</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>56</v>
@@ -7280,7 +6929,7 @@
         <v>57</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AW2" s="6"/>
       <c r="AX2" s="6" t="s">
@@ -7290,7 +6939,7 @@
         <v>58</v>
       </c>
       <c r="AZ2" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6" t="s">
@@ -7306,1520 +6955,548 @@
         <v>61</v>
       </c>
       <c r="BF2" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
       <c r="AL3" s="6"/>
-      <c r="AM3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS3" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV3" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
+      <c r="AR3" s="6"/>
+      <c r="AS3" s="6"/>
+      <c r="AT3" s="6"/>
+      <c r="AU3" s="6"/>
+      <c r="AV3" s="6"/>
       <c r="AW3" s="6"/>
-      <c r="AX3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX3" s="6"/>
+      <c r="AY3" s="6"/>
+      <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
-      <c r="BB3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF3" s="6" t="s">
-        <v>101</v>
-      </c>
+      <c r="BB3" s="6"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="6"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V4" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC4" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK4" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
       <c r="AL4" s="6"/>
-      <c r="AM4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS4" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV4" s="6" t="s">
-        <v>108</v>
-      </c>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
       <c r="AW4" s="6"/>
-      <c r="AX4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ4" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX4" s="6"/>
+      <c r="AY4" s="6"/>
+      <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
-      <c r="BB4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF4" s="6" t="s">
-        <v>109</v>
-      </c>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V5" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC5" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
       <c r="AL5" s="6"/>
-      <c r="AM5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS5" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV5" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
       <c r="AW5" s="6"/>
-      <c r="AX5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ5" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX5" s="6"/>
+      <c r="AY5" s="6"/>
+      <c r="AZ5" s="6"/>
       <c r="BA5" s="6"/>
-      <c r="BB5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF5" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="BB5" s="6"/>
+      <c r="BC5" s="6"/>
+      <c r="BD5" s="6"/>
+      <c r="BE5" s="6"/>
+      <c r="BF5" s="6"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V6" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC6" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS6" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV6" s="6" t="s">
-        <v>124</v>
-      </c>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
       <c r="AW6" s="6"/>
-      <c r="AX6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ6" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX6" s="6"/>
+      <c r="AY6" s="6"/>
+      <c r="AZ6" s="6"/>
       <c r="BA6" s="6"/>
-      <c r="BB6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF6" s="6" t="s">
-        <v>125</v>
-      </c>
+      <c r="BB6" s="6"/>
+      <c r="BC6" s="6"/>
+      <c r="BD6" s="6"/>
+      <c r="BE6" s="6"/>
+      <c r="BF6" s="6"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V7" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK7" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
       <c r="AL7" s="6"/>
-      <c r="AM7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS7" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV7" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
       <c r="AW7" s="6"/>
-      <c r="AX7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ7" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
+      <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
-      <c r="BB7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF7" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="6"/>
+      <c r="BE7" s="6"/>
+      <c r="BF7" s="6"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V8" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC8" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK8" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS8" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV8" s="6" t="s">
-        <v>140</v>
-      </c>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
       <c r="AW8" s="6"/>
-      <c r="AX8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ8" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF8" s="6" t="s">
-        <v>141</v>
-      </c>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>144</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V9" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK9" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS9" s="6">
-        <v>323905952</v>
-      </c>
-      <c r="AT9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV9" s="6" t="s">
-        <v>148</v>
-      </c>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
       <c r="AW9" s="6"/>
-      <c r="AX9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ9" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX9" s="6"/>
+      <c r="AY9" s="6"/>
+      <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
-      <c r="BB9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF9" s="6" t="s">
-        <v>149</v>
-      </c>
+      <c r="BB9" s="6"/>
+      <c r="BC9" s="6"/>
+      <c r="BD9" s="6"/>
+      <c r="BE9" s="6"/>
+      <c r="BF9" s="6"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V10" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z10" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA10" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK10" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
-      <c r="AM10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS10" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV10" s="6" t="s">
-        <v>156</v>
-      </c>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
       <c r="AW10" s="6"/>
-      <c r="AX10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ10" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX10" s="6"/>
+      <c r="AY10" s="6"/>
+      <c r="AZ10" s="6"/>
       <c r="BA10" s="6"/>
-      <c r="BB10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF10" s="6" t="s">
-        <v>157</v>
-      </c>
+      <c r="BB10" s="6"/>
+      <c r="BC10" s="6"/>
+      <c r="BD10" s="6"/>
+      <c r="BE10" s="6"/>
+      <c r="BF10" s="6"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>160</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V11" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA11" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC11" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF11" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK11" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS11" s="6">
-        <v>324101096</v>
-      </c>
-      <c r="AT11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV11" s="6" t="s">
-        <v>164</v>
-      </c>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="6"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
+      <c r="AV11" s="6"/>
       <c r="AW11" s="6"/>
-      <c r="AX11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ11" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX11" s="6"/>
+      <c r="AY11" s="6"/>
+      <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
-      <c r="BB11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF11" s="6" t="s">
-        <v>165</v>
-      </c>
+      <c r="BB11" s="6"/>
+      <c r="BC11" s="6"/>
+      <c r="BD11" s="6"/>
+      <c r="BE11" s="6"/>
+      <c r="BF11" s="6"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -13757,7 +12434,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:BF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:BF58"/>
     </sheetView>
   </sheetViews>
@@ -13938,10 +12615,10 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>166</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3">
-        <v>44621</v>
+        <v>44628</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -13962,13 +12639,13 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>167</v>
+        <v>86</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -13978,31 +12655,31 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>168</v>
+        <v>87</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>49</v>
@@ -14011,7 +12688,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43565</v>
+        <v>43742</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -14023,28 +12700,28 @@
         <v>31028</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AH2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AL2" s="6"/>
       <c r="AM2" s="6" t="s">
@@ -14066,7 +12743,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="6">
-        <v>648173052</v>
+        <v>3381473468</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>55</v>
@@ -14075,7 +12752,7 @@
         <v>63</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="AW2" s="6"/>
       <c r="AX2" s="6" t="s">
@@ -14085,7 +12762,7 @@
         <v>58</v>
       </c>
       <c r="AZ2" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6" t="s">
@@ -14101,1520 +12778,548 @@
         <v>61</v>
       </c>
       <c r="BF2" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
       <c r="AL3" s="6"/>
-      <c r="AM3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS3" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV3" s="6" t="s">
-        <v>173</v>
-      </c>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
+      <c r="AR3" s="6"/>
+      <c r="AS3" s="6"/>
+      <c r="AT3" s="6"/>
+      <c r="AU3" s="6"/>
+      <c r="AV3" s="6"/>
       <c r="AW3" s="6"/>
-      <c r="AX3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX3" s="6"/>
+      <c r="AY3" s="6"/>
+      <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
-      <c r="BB3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF3" s="6" t="s">
-        <v>101</v>
-      </c>
+      <c r="BB3" s="6"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="6"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V4" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC4" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK4" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
       <c r="AL4" s="6"/>
-      <c r="AM4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS4" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV4" s="6" t="s">
-        <v>177</v>
-      </c>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
       <c r="AW4" s="6"/>
-      <c r="AX4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ4" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX4" s="6"/>
+      <c r="AY4" s="6"/>
+      <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
-      <c r="BB4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF4" s="6" t="s">
-        <v>109</v>
-      </c>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V5" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC5" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
       <c r="AL5" s="6"/>
-      <c r="AM5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS5" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV5" s="6" t="s">
-        <v>181</v>
-      </c>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
       <c r="AW5" s="6"/>
-      <c r="AX5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ5" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX5" s="6"/>
+      <c r="AY5" s="6"/>
+      <c r="AZ5" s="6"/>
       <c r="BA5" s="6"/>
-      <c r="BB5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF5" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="BB5" s="6"/>
+      <c r="BC5" s="6"/>
+      <c r="BD5" s="6"/>
+      <c r="BE5" s="6"/>
+      <c r="BF5" s="6"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V6" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC6" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS6" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV6" s="6" t="s">
-        <v>185</v>
-      </c>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
       <c r="AW6" s="6"/>
-      <c r="AX6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ6" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX6" s="6"/>
+      <c r="AY6" s="6"/>
+      <c r="AZ6" s="6"/>
       <c r="BA6" s="6"/>
-      <c r="BB6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF6" s="6" t="s">
-        <v>125</v>
-      </c>
+      <c r="BB6" s="6"/>
+      <c r="BC6" s="6"/>
+      <c r="BD6" s="6"/>
+      <c r="BE6" s="6"/>
+      <c r="BF6" s="6"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V7" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK7" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
       <c r="AL7" s="6"/>
-      <c r="AM7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS7" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV7" s="6" t="s">
-        <v>189</v>
-      </c>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
       <c r="AW7" s="6"/>
-      <c r="AX7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ7" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
+      <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
-      <c r="BB7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF7" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="6"/>
+      <c r="BE7" s="6"/>
+      <c r="BF7" s="6"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V8" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC8" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK8" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS8" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV8" s="6" t="s">
-        <v>193</v>
-      </c>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
       <c r="AW8" s="6"/>
-      <c r="AX8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ8" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
-      <c r="BB8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF8" s="6" t="s">
-        <v>141</v>
-      </c>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B9" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>144</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V9" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK9" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS9" s="6">
-        <v>647754188</v>
-      </c>
-      <c r="AT9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV9" s="6" t="s">
-        <v>197</v>
-      </c>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
       <c r="AW9" s="6"/>
-      <c r="AX9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ9" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX9" s="6"/>
+      <c r="AY9" s="6"/>
+      <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
-      <c r="BB9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF9" s="6" t="s">
-        <v>149</v>
-      </c>
+      <c r="BB9" s="6"/>
+      <c r="BC9" s="6"/>
+      <c r="BD9" s="6"/>
+      <c r="BE9" s="6"/>
+      <c r="BF9" s="6"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V10" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z10" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA10" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK10" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
-      <c r="AM10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS10" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV10" s="6" t="s">
-        <v>201</v>
-      </c>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
       <c r="AW10" s="6"/>
-      <c r="AX10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ10" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX10" s="6"/>
+      <c r="AY10" s="6"/>
+      <c r="AZ10" s="6"/>
       <c r="BA10" s="6"/>
-      <c r="BB10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF10" s="6" t="s">
-        <v>157</v>
-      </c>
+      <c r="BB10" s="6"/>
+      <c r="BC10" s="6"/>
+      <c r="BD10" s="6"/>
+      <c r="BE10" s="6"/>
+      <c r="BF10" s="6"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" s="3">
-        <v>44621</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>160</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V11" s="6">
-        <v>2008</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>43565</v>
-      </c>
-      <c r="AA11" s="3">
-        <v>45046</v>
-      </c>
-      <c r="AB11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC11" s="6">
-        <v>31028</v>
-      </c>
-      <c r="AD11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF11" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK11" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS11" s="6">
-        <v>648144288</v>
-      </c>
-      <c r="AT11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV11" s="6" t="s">
-        <v>205</v>
-      </c>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="6"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
+      <c r="AV11" s="6"/>
       <c r="AW11" s="6"/>
-      <c r="AX11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ11" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AX11" s="6"/>
+      <c r="AY11" s="6"/>
+      <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
-      <c r="BB11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF11" s="6" t="s">
-        <v>165</v>
-      </c>
+      <c r="BB11" s="6"/>
+      <c r="BC11" s="6"/>
+      <c r="BD11" s="6"/>
+      <c r="BE11" s="6"/>
+      <c r="BF11" s="6"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>

</xml_diff>

<commit_message>
Serie Caillou celebra la navidad SD y HD 101
</commit_message>
<xml_diff>
--- a/Run_File.xlsx
+++ b/Run_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5E62C3-359B-428A-94ED-0C9AF06F1803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9C381B-7350-462B-8346-7ACEC2681BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
   </bookViews>
@@ -233,76 +233,76 @@
     <t>FileName</t>
   </si>
   <si>
-    <t>EEBOBG101_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEBO6000000000000101</t>
-  </si>
-  <si>
-    <t>Serie Bob Construye, construcciones ecológicas</t>
-  </si>
-  <si>
-    <t>Bob Construye, construcciones ecológicasT01EP01</t>
-  </si>
-  <si>
-    <t>Bob Construye, construcciones ecológicas T01 EP01</t>
-  </si>
-  <si>
-    <t>Edye presenta: Bob está de vuelta en el sitio. Únete a Bob mientras te muestra el increíble mundo de hogares ecológicos y centros de reciclaje.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Bob está de vuelta en el sitio. Únase a Bob mientras le muestra el asombroso mundo de las casas ecológicas y los centros de reciclaje y aprenda cómo las cosas que tira pueden usarse para hacer algo nuevo. Vea cómo todos pueden unirse y divertirse construyendo casas ecológicas.</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>01:00:05</t>
+    <t>EECAIL101_SD_ADI.XML</t>
   </si>
   <si>
-    <t>01:00</t>
+    <t>EECA6000000000000101</t>
   </si>
   <si>
-    <t>Infantil/Bob Construye, construcciones ecológicas</t>
+    <t>Serie Caillou celebra la navidad</t>
   </si>
   <si>
-    <t>Bob Construye, construcciones ecológicas</t>
+    <t>Caillou celebra la navidadT01EP01</t>
   </si>
   <si>
-    <t>UK</t>
+    <t>Caillou celebra la navidad T01 EP01</t>
   </si>
   <si>
-    <t>Neil Morrissey</t>
+    <t>Edye presenta: Diviértete junto al pequeño Caillou y descubre el milagro de la Navidad.</t>
   </si>
   <si>
-    <t>HIT Ent. Ltd Keith</t>
+    <t>Edye presenta: Es invierno y en la casa del pequeño Caillou se preparan para pasar una hermosa Navidad. Diviértete aprendiendo junto al curioso niño de cuatro años sobre las fiestas y descubre el milagro del amor y la amistad.</t>
   </si>
   <si>
-    <t>Morrissey Neil</t>
+    <t>01:11:00</t>
   </si>
   <si>
-    <t>Little, Brian</t>
+    <t>01:11</t>
   </si>
   <si>
-    <t>EEBOBG101.mpg</t>
+    <t>Infantil/Caillou celebra la navidad</t>
   </si>
   <si>
-    <t>EEBOBG1_box.jpg</t>
+    <t>Caillou celebra la navidad</t>
   </si>
   <si>
-    <t>EEBOBG101_land.jpg</t>
+    <t>CA</t>
   </si>
   <si>
-    <t>EEBOBG101_HD_ADI.XML</t>
+    <t>Annie Bovaird</t>
   </si>
   <si>
-    <t>EEBO7000000000000101</t>
+    <t>Caillou Prod. Inc.</t>
   </si>
   <si>
-    <t>Bob Construye, construcciones ecológicas T01 EP01 HD</t>
+    <t>Bovaird Annie</t>
   </si>
   <si>
-    <t>EEBOBG101.ts</t>
+    <t>Rijgersberg, Nick</t>
+  </si>
+  <si>
+    <t>EECAIL101.mpg</t>
+  </si>
+  <si>
+    <t>EECAIL1_box.jpg</t>
+  </si>
+  <si>
+    <t>EECAIL101_land.jpg</t>
+  </si>
+  <si>
+    <t>EECAIL101_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EECA7000000000000101</t>
+  </si>
+  <si>
+    <t>Caillou celebra la navidad T01 EP01 HD</t>
+  </si>
+  <si>
+    <t>EECAIL101.ts</t>
   </si>
 </sst>
 </file>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3">
         <v>44628</v>
@@ -6816,13 +6816,13 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -6832,19 +6832,19 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>73</v>
@@ -6853,7 +6853,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -6865,7 +6865,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43742</v>
+        <v>43189</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -6920,7 +6920,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="6">
-        <v>1690768412</v>
+        <v>2040386748</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>56</v>
@@ -12435,7 +12435,7 @@
   <dimension ref="A1:BF58"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BF58"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12642,10 +12642,10 @@
         <v>86</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -12661,13 +12661,13 @@
         <v>48</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>73</v>
@@ -12676,7 +12676,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -12688,7 +12688,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43742</v>
+        <v>43189</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -12743,7 +12743,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="6">
-        <v>3381473468</v>
+        <v>4080715968</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Serie Los pies mágicos de Franny SD y HD 301-313
</commit_message>
<xml_diff>
--- a/Run_File.xlsx
+++ b/Run_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288D9FA-E93D-43C9-9265-5D320C3626BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B30BE1F-F9DE-4DC4-93E5-DE4AB8AD45E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="247">
   <si>
     <t>Creation_Date</t>
   </si>
@@ -233,457 +233,550 @@
     <t>TV-Y</t>
   </si>
   <si>
-    <t>EEMOMS231_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000231</t>
-  </si>
-  <si>
-    <t>Serie Matemonstruos</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP31</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP31</t>
-  </si>
-  <si>
-    <t>EP 31</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón aprende a hacer una regla para medir cubos y ayudar al Señor Enojón.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón ayuda al Señor Enojón a medir los cubos de limo para que quepan en las cajas. Para ello, aprenden a hacer una regla, es decir, una línea de números que les permite calcular la longitud de los cubos.</t>
-  </si>
-  <si>
-    <t>00:12:06</t>
-  </si>
-  <si>
-    <t>00:12</t>
-  </si>
-  <si>
-    <t>Infantil/Matemonstruos</t>
-  </si>
-  <si>
-    <t>Matemonstruos</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Cory Doran</t>
-  </si>
-  <si>
-    <t>DHX Monsters Inc</t>
-  </si>
-  <si>
-    <t>Doran Cory</t>
-  </si>
-  <si>
-    <t>Gordon, William</t>
-  </si>
-  <si>
-    <t>EEMOMS231.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS2_box.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS231_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS232_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000232</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP32</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP32</t>
-  </si>
-  <si>
-    <t>EP 32</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos ayudan a completar el ramo de flores de una novia el día de su boda.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos ayudan a un monstruo en el día de su boda. La novia necesita más flores para su ramo. Juntos aprenden que el número de las cosas siempre permanece igual aunque se les aumente el tamaño.</t>
-  </si>
-  <si>
-    <t>00:11:02</t>
-  </si>
-  <si>
-    <t>00:11</t>
-  </si>
-  <si>
-    <t>EEMOMS232.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS232_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS233_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000233</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP33</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP33</t>
-  </si>
-  <si>
-    <t>EP 33</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón le enseña al Monstruo Granjero a calcular la cantidad de dientes de sus plantas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón le enseña al Monstruo Granjero a contar objetos en movimiento. Esto le sirve para calcular la cantidad de dientes que tendrá cada planta carnívora que está cultivando.</t>
-  </si>
-  <si>
-    <t>EEMOMS233.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS233_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS234_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000234</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP34</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP34</t>
-  </si>
-  <si>
-    <t>EP 34</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos ayudan a un escultor muy torpe a terminar su última escultura.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos ayudan a un escultor muy torpe a terminar su última monstruosa escultura, al enseñarle que el volumen del objeto no afecta su forma.</t>
-  </si>
-  <si>
-    <t>00:09:04</t>
-  </si>
-  <si>
-    <t>00:09</t>
-  </si>
-  <si>
-    <t>EEMOMS234.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS234_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS235_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000235</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP35</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP35</t>
-  </si>
-  <si>
-    <t>EP 35</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos comparan dos plantas para ver cuál recibió mayor cantidad de agua.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Comparando dos objetos, el escuadrón puede determinar si uno tiene mayor cantidad de materia que el otro. En este caso, si la cantidad de agua que se le dio a una planta es menor que la que se le dio a otra.</t>
-  </si>
-  <si>
-    <t>00:11:06</t>
-  </si>
-  <si>
-    <t>EEMOMS235.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS235_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS236_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000236</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP36</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP36</t>
-  </si>
-  <si>
-    <t>EP 36</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón ayuda a un monstruo dormilón a fabricar una cama, pero antes le enseña a sumar.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón ayuda a un monstruo dormilón a seguir las instrucciones para fabricar una cama de compost. Para ello, deben enseñarle que la suma indica que dos o más objetos están juntos.</t>
-  </si>
-  <si>
-    <t>00:11:46</t>
-  </si>
-  <si>
-    <t>EEMOMS236.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS236_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS237_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000237</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP37</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP37</t>
-  </si>
-  <si>
-    <t>EP 37</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón utiliza la resta para ayudar a unos pequeños monstruos a montar un vehículo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Unos pequeños monstruos quieren andar en el nuevo Monstruo Juego, pero todos no caben en el vehículo. El escuadrón usa la resta para armar dos grupos y que quepan perfectos en el auto.</t>
-  </si>
-  <si>
-    <t>00:11:40</t>
-  </si>
-  <si>
-    <t>EEMOMS237.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS237_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS238_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000238</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP38</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP38</t>
-  </si>
-  <si>
-    <t>EP 38</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos deben encajar todas las llaves dentro de una caja para desbloquearla.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos aprender sobre cómo encajan las piezas, mientras ayudan a un monstruo a desbloquear una cajita de sorpresas. Para lograrlo deben colocar de manera correcta todas las llaves dentro de los orificios de la caja.</t>
-  </si>
-  <si>
-    <t>00:11:12</t>
-  </si>
-  <si>
-    <t>EEMOMS238.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS238_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS239_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000239</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP39</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP39</t>
-  </si>
-  <si>
-    <t>EP 39</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos aprenden a contar de manera regresiva y ayudan al Monstruo Bromista.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los Matemonstruos aprenden a contar de manera regresiva siguiendo la misma línea de números con la que cuentan para adelante. De esta manera, cuentan del cinco al uno y ayudan al Monstruo Bromista a completar su agenda.</t>
-  </si>
-  <si>
-    <t>00:11:28</t>
-  </si>
-  <si>
-    <t>EEMOMS239.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS239_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS240_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO6000000000000240</t>
-  </si>
-  <si>
-    <t>MatemonstruosT02EP40</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP40</t>
-  </si>
-  <si>
-    <t>EP 40</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón ayuda a calmar las aguas entre los pequeños monstruos de la guardería.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El escuadrón ayuda a calmar las aguas entre los pequeños monstruos de la guardería mientras aprenden que dos conjuntos de objetos son iguales si cada uno de ellos se compone del mismo número de cosas.</t>
-  </si>
-  <si>
-    <t>00:11:43</t>
-  </si>
-  <si>
-    <t>EEMOMS240.mpg</t>
-  </si>
-  <si>
-    <t>EEMOMS240_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMOMS231_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000231</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP31 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS231.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS232_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000232</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP32 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS232.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS233_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000233</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP33 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS233.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS234_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000234</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP34 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS234.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS235_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000235</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP35 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS235.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS236_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000236</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP36 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS236.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS237_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000237</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP37 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS237.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS238_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000238</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP38 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS238.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS239_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000239</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP39 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS239.ts</t>
-  </si>
-  <si>
-    <t>EEMOMS240_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMO7000000000000240</t>
-  </si>
-  <si>
-    <t>Matemonstruos T02 EP40 HD</t>
-  </si>
-  <si>
-    <t>EEMOMS240.ts</t>
+    <t>EEFNFT301_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000301</t>
+  </si>
+  <si>
+    <t>Serie Los pies mágicos de Franny</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP01</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP01</t>
+  </si>
+  <si>
+    <t>EP 01</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny crea una escalera para que Leo, el ratón, pueda alcanzar la lente del observatorio.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En un observatorio de Hawai, Franny se encuentra con un ratón apasionado por la astronomía que debido a su pequeño tamaño nunca ha podido alcanzar la lente del telescopio.Franny crea una escalera, y por primera vez el ratón ve anillos de Saturno.</t>
+  </si>
+  <si>
+    <t>00:21:47</t>
+  </si>
+  <si>
+    <t>00:22</t>
+  </si>
+  <si>
+    <t>Infantil/Los pies mágicos de Franny</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Phoebe McAuley, George Buza</t>
+  </si>
+  <si>
+    <t>Decode Franny Prod.</t>
+  </si>
+  <si>
+    <t>McAuley Phoebe, Buza George</t>
+  </si>
+  <si>
+    <t>Wilmot, Frederick Marcello</t>
+  </si>
+  <si>
+    <t>EEFNFT301.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT3_box.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT301_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT302_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000302</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP02</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP02</t>
+  </si>
+  <si>
+    <t>EP 02</t>
+  </si>
+  <si>
+    <t>Edye presenta: En Jamaica Franny y su amigo descubren que la marea se llevó su castillo de arena.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny visita a un amigo en Jamaica, donde construyen un castillo de arena en la playa.Después de un rápido viaje al mercado, su castillo ya no está, pero jugando a los detectives, se dieron cuenta que la marea se llevó su castillo de arena.</t>
+  </si>
+  <si>
+    <t>00:21:48</t>
+  </si>
+  <si>
+    <t>EEFNFT302.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT302_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT303_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000303</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP03</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP03</t>
+  </si>
+  <si>
+    <t>EP 03</t>
+  </si>
+  <si>
+    <t>Edye presenta: Al ver cómo los egipcios usan el papiro, Franny encuentra una solución para una princesa.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En el antiguo Egipto, Franny visita a una princesa que quiere agregar un jeroglífico al muro familiar pero antes debe practicar escribir el nombre. Al ver cómo los egipcios usan el papiro, Franny encuentra una solución para la princesa.</t>
+  </si>
+  <si>
+    <t>EEFNFT303.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT303_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT304_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000304</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP04</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP04</t>
+  </si>
+  <si>
+    <t>EP 04</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny ayuda a su amiga a buscar a su hermano usando el olfato y el tacto.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny ayuda a su amiga a buscar a su hermano jugando a las econdidas de noche, pero el ruido y la poca visibilidad lo hacen muy difícil. Sabiendo que su hermano come miel, Franny piensa que usando el olfato y el tacto lo pueden encontrar.</t>
+  </si>
+  <si>
+    <t>EEFNFT304.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT304_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT305_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000305</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP05</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP05</t>
+  </si>
+  <si>
+    <t>EP 05</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny viaja en un globo aerostático y ayuda a una mariposa a volar a México.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny viaja en un globo aerostático y ayuda a una mariposa a volar a México para su hibernación.Al ver cómo el globo sube con aire caliente y baja con aire frío, Franny sugiere que la mariposa use aire caliente para ayudarla a volar.</t>
+  </si>
+  <si>
+    <t>00:21:46</t>
+  </si>
+  <si>
+    <t>EEFNFT305.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT305_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT306_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000306</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP06</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP06</t>
+  </si>
+  <si>
+    <t>EP 06</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny conoce a un amigo en la Antártida y descubre el lugar perfecto para que anide su huevo.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En la Antártida, Franny conoce a un pingüino novato ciudando huevos que está agotado de proteger su huevo del frío con sus alas. Franny descubre el lugar perfecto y cálido para que Prewitt anide su huevo: debajo del estómago y encima de sus pies.</t>
+  </si>
+  <si>
+    <t>EEFNFT306.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT306_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT307_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000307</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP07</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP07</t>
+  </si>
+  <si>
+    <t>EP 07</t>
+  </si>
+  <si>
+    <t>Edye presenta: En una boda tradicional de la India, Franny crea una bufanda nueva para su amigo.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En una boda tradicional de la India, Franny conoce a un nuevo amigo, un niño cuya bufanda verde translúcida se daña en una planta.Franny tiene una solución y coloca una bufanda amarilla translúcida sobre una azul y crea una verde.</t>
+  </si>
+  <si>
+    <t>EEFNFT307.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT307_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT308_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000308</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP08</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP08</t>
+  </si>
+  <si>
+    <t>EP 08</t>
+  </si>
+  <si>
+    <t>Edye presenta: En un ballet, Franny conoce a Lila, quien da vida a una galleta de jengibre en El Cascanueces.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Tras bambalinas de un ballet, Franny conoce a Lila, quien hace el papel de una galleta de jengibre en El Cascanueces. Lila le muestra a Franny el lugar donde ensayan, dónde va la orquesta y la zona donde está el árbol más grande que haya visto.</t>
+  </si>
+  <si>
+    <t>EEFNFT308.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT308_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT309_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000309</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP09</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP09</t>
+  </si>
+  <si>
+    <t>EP 09</t>
+  </si>
+  <si>
+    <t>Edye presenta: En Nueva Zelanda, Franny convive con Iwi, un ave kiwi que le enseña todo sobre su especie.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Franny visita Nueva Zelanda y conoce a Iwi, un ave kiwi que cuida a un pequeño que pronto saldrá del huevo. Cuando la madre llega a cumplir con sus deberes, Iwi le enseña a Franny el área y ella aprende todo sobre los Iwi ¡y prueba deliciosos kiwis!</t>
+  </si>
+  <si>
+    <t>EEFNFT309.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT309_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT310_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000310</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP10</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP10</t>
+  </si>
+  <si>
+    <t>EP 10</t>
+  </si>
+  <si>
+    <t>Edye presenta: El joven astronauta Cosmo le muestra a Fanny su estación espacial y ella flota por todos lados.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En el espacio, Franny conoce a Cosmo, un joven astronauta que le muestra la estación espacial internacional. Ella experimenta la falta de gravedad pues flota en todos lados; también aprende cómo comer, hacer ejercicio y trabajar en el espacio.</t>
+  </si>
+  <si>
+    <t>EEFNFT310.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT310_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT311_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000311</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP11</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP11</t>
+  </si>
+  <si>
+    <t>EP 11</t>
+  </si>
+  <si>
+    <t>Edye presenta: En China, Franny conoce a Ling, quien le dice todo sobre sus amigos Panda: Ko ko, Boo y Nana.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En las montañas de China, Franny conoce a Ling, una joven con amigos Panda: Ko ko, Boo y Nana. Franny aprende todo sobre los osos panda y su comida favorita: el bambú. Cuando comienza a hacer viento, Ling decide que los pandas regresen a su refugio.</t>
+  </si>
+  <si>
+    <t>EEFNFT311.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT311_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT312_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000312</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP12</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP12</t>
+  </si>
+  <si>
+    <t>EP 12</t>
+  </si>
+  <si>
+    <t>Edye presenta: En islas Galápagos, Franny aconseja a la tortuga Tomás ser él mismo para conseguir amigos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En islas Galápagos, Franny conoce a dos tortugas: Tomás y Tilly. A Tomás le gustaría ser amigo de Tilly e intenta varias formas de llamar su atención, pero sus esfuerzos no tienen éxito. Franny le sugiere que sólo hable con ella y sea él mismo.</t>
+  </si>
+  <si>
+    <t>EEFNFT312.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT312_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT313_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN6000000000000313</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de FrannyT03EP13</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP13</t>
+  </si>
+  <si>
+    <t>EP 13</t>
+  </si>
+  <si>
+    <t>Edye presenta: Walter y Mac son dos monos de Gibraltar que le enseñan a Franny el valor de una gran amistad.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En Gibraltar, Franny conoce a Walter y Mac. Walter es un mono tímido y quiere ser amigo de Mac, el simio más popular y extrovertido, pero cree que no tiene tiempo para él. En un viaje a las cuevas, Walter sabe que Mac teme a las sombras y le ayuda.</t>
+  </si>
+  <si>
+    <t>EEFNFT313.mpg</t>
+  </si>
+  <si>
+    <t>EEFNFT313_land.jpg</t>
+  </si>
+  <si>
+    <t>EEFNFT301_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000301</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP01 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT301.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT302_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000302</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP02 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT302.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT303_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000303</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP03 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT303.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT304_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000304</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP04 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT304.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT305_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000305</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP05 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT305.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT306_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000306</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP06 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT306.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT307_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000307</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP07 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT307.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT308_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000308</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP08 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT308.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT309_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000309</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP09 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT309.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT310_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000310</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP10 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT310.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT311_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000311</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP11 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT311.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT312_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000312</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP12 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT312.ts</t>
+  </si>
+  <si>
+    <t>EEFNFT313_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEFN7000000000000313</t>
+  </si>
+  <si>
+    <t>Los pies mágicos de Franny T03 EP13 HD</t>
+  </si>
+  <si>
+    <t>EEFNFT313.ts</t>
   </si>
 </sst>
 </file>
@@ -7176,7 +7269,7 @@
         <v>65</v>
       </c>
       <c r="B2" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -7234,7 +7327,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -7246,7 +7339,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -7301,7 +7394,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>340931984</v>
+        <v>613271792</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>55</v>
@@ -7344,7 +7437,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>43</v>
@@ -7399,10 +7492,10 @@
         <v>92</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V3" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>75</v>
@@ -7414,7 +7507,7 @@
         <v>44</v>
       </c>
       <c r="Z3" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA3" s="3">
         <v>45046</v>
@@ -7469,7 +7562,7 @@
         <v>54</v>
       </c>
       <c r="AS3" s="6">
-        <v>320443368</v>
+        <v>613406588</v>
       </c>
       <c r="AT3" s="6" t="s">
         <v>55</v>
@@ -7478,7 +7571,7 @@
         <v>56</v>
       </c>
       <c r="AV3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AW3" s="6"/>
       <c r="AX3" s="6" t="s">
@@ -7504,15 +7597,15 @@
         <v>60</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>43</v>
@@ -7533,13 +7626,13 @@
         <v>46</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="6" t="s">
@@ -7549,16 +7642,16 @@
         <v>47</v>
       </c>
       <c r="O4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>64</v>
@@ -7570,7 +7663,7 @@
         <v>74</v>
       </c>
       <c r="V4" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>75</v>
@@ -7582,7 +7675,7 @@
         <v>44</v>
       </c>
       <c r="Z4" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA4" s="3">
         <v>45046</v>
@@ -7637,7 +7730,7 @@
         <v>54</v>
       </c>
       <c r="AS4" s="6">
-        <v>340931984</v>
+        <v>613452460</v>
       </c>
       <c r="AT4" s="6" t="s">
         <v>55</v>
@@ -7646,7 +7739,7 @@
         <v>56</v>
       </c>
       <c r="AV4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AW4" s="6"/>
       <c r="AX4" s="6" t="s">
@@ -7672,15 +7765,15 @@
         <v>60</v>
       </c>
       <c r="BF4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>43</v>
@@ -7701,13 +7794,13 @@
         <v>46</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6" t="s">
@@ -7717,28 +7810,28 @@
         <v>47</v>
       </c>
       <c r="O5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="V5" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>75</v>
@@ -7750,7 +7843,7 @@
         <v>44</v>
       </c>
       <c r="Z5" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA5" s="3">
         <v>45046</v>
@@ -7805,7 +7898,7 @@
         <v>54</v>
       </c>
       <c r="AS5" s="6">
-        <v>274408372</v>
+        <v>613346428</v>
       </c>
       <c r="AT5" s="6" t="s">
         <v>55</v>
@@ -7814,7 +7907,7 @@
         <v>56</v>
       </c>
       <c r="AV5" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AW5" s="6"/>
       <c r="AX5" s="6" t="s">
@@ -7840,15 +7933,15 @@
         <v>60</v>
       </c>
       <c r="BF5" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B6" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>43</v>
@@ -7869,13 +7962,13 @@
         <v>46</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
@@ -7885,28 +7978,28 @@
         <v>47</v>
       </c>
       <c r="O6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V6" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>75</v>
@@ -7918,7 +8011,7 @@
         <v>44</v>
       </c>
       <c r="Z6" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA6" s="3">
         <v>45046</v>
@@ -7973,7 +8066,7 @@
         <v>54</v>
       </c>
       <c r="AS6" s="6">
-        <v>312792332</v>
+        <v>613033596</v>
       </c>
       <c r="AT6" s="6" t="s">
         <v>55</v>
@@ -7982,7 +8075,7 @@
         <v>56</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AW6" s="6"/>
       <c r="AX6" s="6" t="s">
@@ -8008,15 +8101,15 @@
         <v>60</v>
       </c>
       <c r="BF6" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B7" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -8037,13 +8130,13 @@
         <v>46</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
@@ -8053,28 +8146,28 @@
         <v>47</v>
       </c>
       <c r="O7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V7" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>75</v>
@@ -8086,7 +8179,7 @@
         <v>44</v>
       </c>
       <c r="Z7" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA7" s="3">
         <v>45046</v>
@@ -8141,7 +8234,7 @@
         <v>54</v>
       </c>
       <c r="AS7" s="6">
-        <v>331663020</v>
+        <v>613033596</v>
       </c>
       <c r="AT7" s="6" t="s">
         <v>55</v>
@@ -8150,7 +8243,7 @@
         <v>56</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AW7" s="6"/>
       <c r="AX7" s="6" t="s">
@@ -8176,15 +8269,15 @@
         <v>60</v>
       </c>
       <c r="BF7" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B8" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>43</v>
@@ -8205,13 +8298,13 @@
         <v>46</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
@@ -8221,28 +8314,28 @@
         <v>47</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V8" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>75</v>
@@ -8254,7 +8347,7 @@
         <v>44</v>
       </c>
       <c r="Z8" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA8" s="3">
         <v>45046</v>
@@ -8309,7 +8402,7 @@
         <v>54</v>
       </c>
       <c r="AS8" s="6">
-        <v>328782860</v>
+        <v>613002012</v>
       </c>
       <c r="AT8" s="6" t="s">
         <v>55</v>
@@ -8318,7 +8411,7 @@
         <v>56</v>
       </c>
       <c r="AV8" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="AW8" s="6"/>
       <c r="AX8" s="6" t="s">
@@ -8344,15 +8437,15 @@
         <v>60</v>
       </c>
       <c r="BF8" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B9" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>43</v>
@@ -8373,13 +8466,13 @@
         <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
@@ -8389,28 +8482,28 @@
         <v>47</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V9" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W9" s="6" t="s">
         <v>75</v>
@@ -8422,7 +8515,7 @@
         <v>44</v>
       </c>
       <c r="Z9" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA9" s="3">
         <v>45046</v>
@@ -8477,7 +8570,7 @@
         <v>54</v>
       </c>
       <c r="AS9" s="6">
-        <v>315506300</v>
+        <v>613002012</v>
       </c>
       <c r="AT9" s="6" t="s">
         <v>55</v>
@@ -8486,7 +8579,7 @@
         <v>56</v>
       </c>
       <c r="AV9" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AW9" s="6"/>
       <c r="AX9" s="6" t="s">
@@ -8512,15 +8605,15 @@
         <v>60</v>
       </c>
       <c r="BF9" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B10" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
@@ -8541,13 +8634,13 @@
         <v>46</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
@@ -8557,28 +8650,28 @@
         <v>47</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V10" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W10" s="6" t="s">
         <v>75</v>
@@ -8590,7 +8683,7 @@
         <v>44</v>
       </c>
       <c r="Z10" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA10" s="3">
         <v>45046</v>
@@ -8645,7 +8738,7 @@
         <v>54</v>
       </c>
       <c r="AS10" s="6">
-        <v>323111276</v>
+        <v>612987724</v>
       </c>
       <c r="AT10" s="6" t="s">
         <v>55</v>
@@ -8654,7 +8747,7 @@
         <v>56</v>
       </c>
       <c r="AV10" s="6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="AW10" s="6"/>
       <c r="AX10" s="6" t="s">
@@ -8680,15 +8773,15 @@
         <v>60</v>
       </c>
       <c r="BF10" s="6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B11" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>43</v>
@@ -8709,13 +8802,13 @@
         <v>46</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
@@ -8725,28 +8818,28 @@
         <v>47</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="U11" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V11" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W11" s="6" t="s">
         <v>75</v>
@@ -8758,7 +8851,7 @@
         <v>44</v>
       </c>
       <c r="Z11" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA11" s="3">
         <v>45046</v>
@@ -8813,7 +8906,7 @@
         <v>54</v>
       </c>
       <c r="AS11" s="6">
-        <v>320847756</v>
+        <v>613033596</v>
       </c>
       <c r="AT11" s="6" t="s">
         <v>55</v>
@@ -8822,7 +8915,7 @@
         <v>56</v>
       </c>
       <c r="AV11" s="6" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AW11" s="6"/>
       <c r="AX11" s="6" t="s">
@@ -8848,188 +8941,512 @@
         <v>60</v>
       </c>
       <c r="BF11" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
+      <c r="M12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V12" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
-      <c r="AP12" s="6"/>
-      <c r="AQ12" s="6"/>
-      <c r="AR12" s="6"/>
-      <c r="AS12" s="6"/>
-      <c r="AT12" s="6"/>
-      <c r="AU12" s="6"/>
-      <c r="AV12" s="6"/>
+      <c r="AM12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS12" s="6">
+        <v>613002012</v>
+      </c>
+      <c r="AT12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="AW12" s="6"/>
-      <c r="AX12" s="6"/>
-      <c r="AY12" s="6"/>
-      <c r="AZ12" s="6"/>
+      <c r="AX12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ12" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="6"/>
-      <c r="BC12" s="6"/>
-      <c r="BD12" s="6"/>
-      <c r="BE12" s="6"/>
-      <c r="BF12" s="6"/>
+      <c r="BB12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>179</v>
+      </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
+      <c r="M13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V13" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL13" s="6"/>
-      <c r="AM13" s="6"/>
-      <c r="AN13" s="6"/>
-      <c r="AO13" s="6"/>
-      <c r="AP13" s="6"/>
-      <c r="AQ13" s="6"/>
-      <c r="AR13" s="6"/>
-      <c r="AS13" s="6"/>
-      <c r="AT13" s="6"/>
-      <c r="AU13" s="6"/>
-      <c r="AV13" s="6"/>
+      <c r="AM13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS13" s="6">
+        <v>613033596</v>
+      </c>
+      <c r="AT13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV13" s="6" t="s">
+        <v>184</v>
+      </c>
       <c r="AW13" s="6"/>
-      <c r="AX13" s="6"/>
-      <c r="AY13" s="6"/>
-      <c r="AZ13" s="6"/>
+      <c r="AX13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ13" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA13" s="6"/>
-      <c r="BB13" s="6"/>
-      <c r="BC13" s="6"/>
-      <c r="BD13" s="6"/>
-      <c r="BE13" s="6"/>
-      <c r="BF13" s="6"/>
+      <c r="BB13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF13" s="6" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>188</v>
+      </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V14" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-      <c r="AO14" s="6"/>
-      <c r="AP14" s="6"/>
-      <c r="AQ14" s="6"/>
-      <c r="AR14" s="6"/>
-      <c r="AS14" s="6"/>
-      <c r="AT14" s="6"/>
-      <c r="AU14" s="6"/>
-      <c r="AV14" s="6"/>
+      <c r="AM14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS14" s="6">
+        <v>613033596</v>
+      </c>
+      <c r="AT14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV14" s="6" t="s">
+        <v>193</v>
+      </c>
       <c r="AW14" s="6"/>
-      <c r="AX14" s="6"/>
-      <c r="AY14" s="6"/>
-      <c r="AZ14" s="6"/>
+      <c r="AX14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ14" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA14" s="6"/>
-      <c r="BB14" s="6"/>
-      <c r="BC14" s="6"/>
-      <c r="BD14" s="6"/>
-      <c r="BE14" s="6"/>
-      <c r="BF14" s="6"/>
+      <c r="BB14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF14" s="6" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -13968,10 +14385,10 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="B2" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -13992,7 +14409,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>67</v>
@@ -14008,7 +14425,7 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>70</v>
@@ -14029,7 +14446,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -14041,7 +14458,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA2" s="3">
         <v>45046</v>
@@ -14096,7 +14513,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>681806440</v>
+        <v>1226485868</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>54</v>
@@ -14105,7 +14522,7 @@
         <v>62</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="AW2" s="6"/>
       <c r="AX2" s="6" t="s">
@@ -14136,10 +14553,10 @@
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="B3" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>43</v>
@@ -14160,7 +14577,7 @@
         <v>46</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>67</v>
@@ -14176,7 +14593,7 @@
         <v>47</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>89</v>
@@ -14194,10 +14611,10 @@
         <v>92</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V3" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>75</v>
@@ -14209,7 +14626,7 @@
         <v>44</v>
       </c>
       <c r="Z3" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA3" s="3">
         <v>45046</v>
@@ -14264,7 +14681,7 @@
         <v>54</v>
       </c>
       <c r="AS3" s="6">
-        <v>640823380</v>
+        <v>1226755460</v>
       </c>
       <c r="AT3" s="6" t="s">
         <v>54</v>
@@ -14273,7 +14690,7 @@
         <v>62</v>
       </c>
       <c r="AV3" s="6" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="AW3" s="6"/>
       <c r="AX3" s="6" t="s">
@@ -14299,15 +14716,15 @@
         <v>60</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>43</v>
@@ -14328,13 +14745,13 @@
         <v>46</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="6" t="s">
@@ -14344,16 +14761,16 @@
         <v>47</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="P4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>64</v>
@@ -14365,7 +14782,7 @@
         <v>74</v>
       </c>
       <c r="V4" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>75</v>
@@ -14377,7 +14794,7 @@
         <v>44</v>
       </c>
       <c r="Z4" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA4" s="3">
         <v>45046</v>
@@ -14432,7 +14849,7 @@
         <v>54</v>
       </c>
       <c r="AS4" s="6">
-        <v>681806440</v>
+        <v>1226847392</v>
       </c>
       <c r="AT4" s="6" t="s">
         <v>54</v>
@@ -14441,7 +14858,7 @@
         <v>62</v>
       </c>
       <c r="AV4" s="6" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="AW4" s="6"/>
       <c r="AX4" s="6" t="s">
@@ -14467,15 +14884,15 @@
         <v>60</v>
       </c>
       <c r="BF4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="B5" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>43</v>
@@ -14496,13 +14913,13 @@
         <v>46</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6" t="s">
@@ -14512,28 +14929,28 @@
         <v>47</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="P5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="V5" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>75</v>
@@ -14545,7 +14962,7 @@
         <v>44</v>
       </c>
       <c r="Z5" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA5" s="3">
         <v>45046</v>
@@ -14600,7 +15017,7 @@
         <v>54</v>
       </c>
       <c r="AS5" s="6">
-        <v>548753388</v>
+        <v>1226635140</v>
       </c>
       <c r="AT5" s="6" t="s">
         <v>54</v>
@@ -14609,7 +15026,7 @@
         <v>62</v>
       </c>
       <c r="AV5" s="6" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="AW5" s="6"/>
       <c r="AX5" s="6" t="s">
@@ -14635,15 +15052,15 @@
         <v>60</v>
       </c>
       <c r="BF5" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="B6" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>43</v>
@@ -14664,13 +15081,13 @@
         <v>46</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
@@ -14680,28 +15097,28 @@
         <v>47</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V6" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>75</v>
@@ -14713,7 +15130,7 @@
         <v>44</v>
       </c>
       <c r="Z6" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA6" s="3">
         <v>45046</v>
@@ -14768,7 +15185,7 @@
         <v>54</v>
       </c>
       <c r="AS6" s="6">
-        <v>625527136</v>
+        <v>1226003836</v>
       </c>
       <c r="AT6" s="6" t="s">
         <v>54</v>
@@ -14777,7 +15194,7 @@
         <v>62</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="AW6" s="6"/>
       <c r="AX6" s="6" t="s">
@@ -14803,15 +15220,15 @@
         <v>60</v>
       </c>
       <c r="BF6" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="B7" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -14832,13 +15249,13 @@
         <v>46</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
@@ -14848,28 +15265,28 @@
         <v>47</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V7" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>75</v>
@@ -14881,7 +15298,7 @@
         <v>44</v>
       </c>
       <c r="Z7" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA7" s="3">
         <v>45046</v>
@@ -14936,7 +15353,7 @@
         <v>54</v>
       </c>
       <c r="AS7" s="6">
-        <v>663262684</v>
+        <v>1226003836</v>
       </c>
       <c r="AT7" s="6" t="s">
         <v>54</v>
@@ -14945,7 +15362,7 @@
         <v>62</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="AW7" s="6"/>
       <c r="AX7" s="6" t="s">
@@ -14971,15 +15388,15 @@
         <v>60</v>
       </c>
       <c r="BF7" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="B8" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>43</v>
@@ -15000,13 +15417,13 @@
         <v>46</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
@@ -15016,28 +15433,28 @@
         <v>47</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V8" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>75</v>
@@ -15049,7 +15466,7 @@
         <v>44</v>
       </c>
       <c r="Z8" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA8" s="3">
         <v>45046</v>
@@ -15104,7 +15521,7 @@
         <v>54</v>
       </c>
       <c r="AS8" s="6">
-        <v>657508004</v>
+        <v>1225946496</v>
       </c>
       <c r="AT8" s="6" t="s">
         <v>54</v>
@@ -15113,7 +15530,7 @@
         <v>62</v>
       </c>
       <c r="AV8" s="6" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="AW8" s="6"/>
       <c r="AX8" s="6" t="s">
@@ -15139,15 +15556,15 @@
         <v>60</v>
       </c>
       <c r="BF8" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="B9" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>43</v>
@@ -15168,13 +15585,13 @@
         <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
@@ -15184,28 +15601,28 @@
         <v>47</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V9" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W9" s="6" t="s">
         <v>75</v>
@@ -15217,7 +15634,7 @@
         <v>44</v>
       </c>
       <c r="Z9" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA9" s="3">
         <v>45046</v>
@@ -15272,7 +15689,7 @@
         <v>54</v>
       </c>
       <c r="AS9" s="6">
-        <v>630954696</v>
+        <v>1225946496</v>
       </c>
       <c r="AT9" s="6" t="s">
         <v>54</v>
@@ -15281,7 +15698,7 @@
         <v>62</v>
       </c>
       <c r="AV9" s="6" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="AW9" s="6"/>
       <c r="AX9" s="6" t="s">
@@ -15307,15 +15724,15 @@
         <v>60</v>
       </c>
       <c r="BF9" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B10" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
@@ -15336,13 +15753,13 @@
         <v>46</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
@@ -15352,28 +15769,28 @@
         <v>47</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="V10" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W10" s="6" t="s">
         <v>75</v>
@@ -15385,7 +15802,7 @@
         <v>44</v>
       </c>
       <c r="Z10" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA10" s="3">
         <v>45046</v>
@@ -15440,7 +15857,7 @@
         <v>54</v>
       </c>
       <c r="AS10" s="6">
-        <v>646165024</v>
+        <v>1225917920</v>
       </c>
       <c r="AT10" s="6" t="s">
         <v>54</v>
@@ -15449,7 +15866,7 @@
         <v>62</v>
       </c>
       <c r="AV10" s="6" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="AW10" s="6"/>
       <c r="AX10" s="6" t="s">
@@ -15475,15 +15892,15 @@
         <v>60</v>
       </c>
       <c r="BF10" s="6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B11" s="3">
-        <v>44626</v>
+        <v>44625</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>43</v>
@@ -15504,13 +15921,13 @@
         <v>46</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
@@ -15520,28 +15937,28 @@
         <v>47</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="U11" s="5" t="s">
         <v>74</v>
       </c>
       <c r="V11" s="6">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="W11" s="6" t="s">
         <v>75</v>
@@ -15553,7 +15970,7 @@
         <v>44</v>
       </c>
       <c r="Z11" s="3">
-        <v>43742</v>
+        <v>43565</v>
       </c>
       <c r="AA11" s="3">
         <v>45046</v>
@@ -15608,7 +16025,7 @@
         <v>54</v>
       </c>
       <c r="AS11" s="6">
-        <v>641637984</v>
+        <v>1226003836</v>
       </c>
       <c r="AT11" s="6" t="s">
         <v>54</v>
@@ -15617,7 +16034,7 @@
         <v>62</v>
       </c>
       <c r="AV11" s="6" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="AW11" s="6"/>
       <c r="AX11" s="6" t="s">
@@ -15643,188 +16060,512 @@
         <v>60</v>
       </c>
       <c r="BF11" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
+      <c r="M12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V12" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
-      <c r="AP12" s="6"/>
-      <c r="AQ12" s="6"/>
-      <c r="AR12" s="6"/>
-      <c r="AS12" s="6"/>
-      <c r="AT12" s="6"/>
-      <c r="AU12" s="6"/>
-      <c r="AV12" s="6"/>
+      <c r="AM12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS12" s="6">
+        <v>1225946496</v>
+      </c>
+      <c r="AT12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>238</v>
+      </c>
       <c r="AW12" s="6"/>
-      <c r="AX12" s="6"/>
-      <c r="AY12" s="6"/>
-      <c r="AZ12" s="6"/>
+      <c r="AX12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ12" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="6"/>
-      <c r="BC12" s="6"/>
-      <c r="BD12" s="6"/>
-      <c r="BE12" s="6"/>
-      <c r="BF12" s="6"/>
+      <c r="BB12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>179</v>
+      </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
+      <c r="M13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V13" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL13" s="6"/>
-      <c r="AM13" s="6"/>
-      <c r="AN13" s="6"/>
-      <c r="AO13" s="6"/>
-      <c r="AP13" s="6"/>
-      <c r="AQ13" s="6"/>
-      <c r="AR13" s="6"/>
-      <c r="AS13" s="6"/>
-      <c r="AT13" s="6"/>
-      <c r="AU13" s="6"/>
-      <c r="AV13" s="6"/>
+      <c r="AM13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS13" s="6">
+        <v>1226003836</v>
+      </c>
+      <c r="AT13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV13" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="AW13" s="6"/>
-      <c r="AX13" s="6"/>
-      <c r="AY13" s="6"/>
-      <c r="AZ13" s="6"/>
+      <c r="AX13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ13" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA13" s="6"/>
-      <c r="BB13" s="6"/>
-      <c r="BC13" s="6"/>
-      <c r="BD13" s="6"/>
-      <c r="BE13" s="6"/>
-      <c r="BF13" s="6"/>
+      <c r="BB13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF13" s="6" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44625</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>188</v>
+      </c>
       <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="V14" s="6">
+        <v>2009</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>43565</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>45046</v>
+      </c>
+      <c r="AB14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>31028</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-      <c r="AO14" s="6"/>
-      <c r="AP14" s="6"/>
-      <c r="AQ14" s="6"/>
-      <c r="AR14" s="6"/>
-      <c r="AS14" s="6"/>
-      <c r="AT14" s="6"/>
-      <c r="AU14" s="6"/>
-      <c r="AV14" s="6"/>
+      <c r="AM14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS14" s="6">
+        <v>1226003836</v>
+      </c>
+      <c r="AT14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV14" s="6" t="s">
+        <v>246</v>
+      </c>
       <c r="AW14" s="6"/>
-      <c r="AX14" s="6"/>
-      <c r="AY14" s="6"/>
-      <c r="AZ14" s="6"/>
+      <c r="AX14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ14" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="BA14" s="6"/>
-      <c r="BB14" s="6"/>
-      <c r="BC14" s="6"/>
-      <c r="BD14" s="6"/>
-      <c r="BE14" s="6"/>
-      <c r="BF14" s="6"/>
+      <c r="BB14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF14" s="6" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>

</xml_diff>

<commit_message>
Serie El día que Henry conoció… SD y HD 401-426
</commit_message>
<xml_diff>
--- a/Run_File.xlsx
+++ b/Run_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121A4E43-2B5A-461E-990A-588E6145E8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674AE2CA-EE9E-4048-9075-E0A1124D5527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
   </bookViews>
   <sheets>
     <sheet name="SD" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="415">
   <si>
     <t>Creation_Date</t>
   </si>
@@ -311,973 +311,976 @@
     <t>EP 26</t>
   </si>
   <si>
-    <t>EEFSAM701_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000701</t>
-  </si>
-  <si>
-    <t>Serie Sam, El Bombero</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP01</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP01</t>
-  </si>
-  <si>
-    <t>Edye presenta: Después de una lección con Penny, Norman se cree el mejor marinero de todos los tiempos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Después de una lección con Penny, Norman cree que es el mejor marinero y, al ignorar una advertencia de Penny, lleva a Dilys a un crucero en el esquife. Mientras tanto, el oficial Steele tiene una nueva cometa que no logra hacer volar.</t>
-  </si>
-  <si>
-    <t>00:10:02</t>
-  </si>
-  <si>
-    <t>00:10</t>
-  </si>
-  <si>
-    <t>Infantil/Sam, El Bombero</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Steven Kynman, David Carling, Su Douglas, Tegwen Tucker</t>
-  </si>
-  <si>
-    <t>Fireman Sam Assoc</t>
-  </si>
-  <si>
-    <t>Kynman Steven, Carling David, Douglas Su, Tucker Tegwen</t>
-  </si>
-  <si>
-    <t>Hibbert, Jerry</t>
-  </si>
-  <si>
-    <t>EEFSAM701.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM7_box.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM701_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM702_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000702</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP02</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP02</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman decide sacar las monedas del pozo de los deseos para reemplazar su monopatín.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman se entristece cuando Trevor atropella accidentalmente su monopatín. Dilys dice que deberá esperar hasta su cumpleaños para obtener otro, pero Norman no quiere esperar tanto y decide sacar las monedas del pozo de los deseos.</t>
-  </si>
-  <si>
-    <t>EEFSAM702.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM702_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM703_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000703</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP03</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP03</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mientras Elvis se recupera de un accidente, el oficial Steele dirige el recate de Mike Flood.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Cuando Elvis se rompe la pierna bailando, comienza a preguntarse si realmente está hecho para ser un bombero. Con Elvis fuera de combate, el oficial Steele está de vuelta en el trabajo y dirige al equipo para rescatar a Mike Flood.</t>
-  </si>
-  <si>
-    <t>EEFSAM703.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM703_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM704_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000704</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP04</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP04</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman y Mandy oyen un grito, es Penny atorada. Los chicos deben hacer algo para ayudarla.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mientras juegan a las escondidas en las montañas, Norman y Mandy escuchan a alguien está pidiendo ayuda: es Penny atorada en el acantilado. Por suerte tienen una luz de bengala para llamar a los bomberos. Ellos vienen al rescate.</t>
-  </si>
-  <si>
-    <t>EEFSAM704.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM704_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM705_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000705</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP05</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP05</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mike tiene problemas con la calabaza que va a presentar en la exhibición de Flores y Vegetales.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Todos están entusiasmados con la exhibición de Flores y Vegetales de Pontypandy, Sam el bombero será el juez. Mike quiere participar con una calabaza que ha estado cultivando, pero al ignorar las recomendaciones de Sam, tiene problemas con su abono.</t>
-  </si>
-  <si>
-    <t>EEFSAM705.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM705_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM706_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000706</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP06</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP06</t>
-  </si>
-  <si>
-    <t>Edye presenta: Trevor conduce el autobús escolar pero se atasca en un pantano.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Trevor lleva a los niños de regreso de un viaje escolar, pero un accidente lleva al autobús a un pantano y se atasca en el lodo. Al anochecer, Trevor ignora los consejos de todos y decide salir a buscar ayuda.</t>
-  </si>
-  <si>
-    <t>EEFSAM706.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM706_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM707_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000707</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP07</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP07</t>
-  </si>
-  <si>
-    <t>Edye presenta: Va a haber un concurso de barbacoas en Pontypandy ¿Quién será el ganador, Trevor o Tom?</t>
-  </si>
-  <si>
-    <t>Edye presenta: Trevor está planeando una barbacoa para los habitantes de Pontypandy y todos esperan sus famosas salchichas. Tom, cocinará también algunos de sus camarones especiales. Los invitados decidirán quién es el campeón de la barbacoa de Pontypandy.</t>
-  </si>
-  <si>
-    <t>EEFSAM707.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM707_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM708_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000708</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP08</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP08</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mientras todos están emocionados por la noche de karaoke, los bomberos realizan un simulacro.</t>
-  </si>
-  <si>
-    <t>Edye presenta: En Pontypandy todos están emocionados por la noche de karaoke. En la estación, Sam y su equipo realizan un simulacro, la tarea es rescatar a una anciana, personificada por el oficial Steele, encerrado en un armario.</t>
-  </si>
-  <si>
-    <t>EEFSAM708.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM708_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM709_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000709</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP09</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP09</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mientras Norman recolecta cangrejos y peces en la playa, Mandy se encuentra una ballena varada.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mandy y Norman se dirigen a la playa desafiándose entre sí para ver quién obtendrá la mejor pesca del día. Norman recolecta cangrejos y peces, pero cuando Mandy se aleja, se encuentra con una ballena varada en la playa.</t>
-  </si>
-  <si>
-    <t>EEFSAM709.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM709_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM710_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000710</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP10</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP10</t>
-  </si>
-  <si>
-    <t>Edye presenta: Al terminar su turno, el bombero Sam usa su tiempo libre para hacer pequeños trabajos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Al terminar su turno, el bombero Sam usa su tiempo libre para hacer pequeños trabajos que se le han acumulado. En la tienda, Mike pone cemento fresco para rellenar las grietas del suelo y luego sube a su escalera para arreglar el desagüe.</t>
-  </si>
-  <si>
-    <t>EEFSAM710.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM710_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM711_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000711</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP11</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP11</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman le pregunta a Sam si Radar podría ser un buen perro pastor para cuidar a sus ovejas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman no puede cuidar solo a Woolly, la oveja y Lambikins, el cordero, por lo que decide pedir ayuda. Al llegar a la estación de bomberos le pregunta a Sam si cree que Radar, el perro de la estación, sería un buen perro pastor.</t>
-  </si>
-  <si>
-    <t>EEFSAM711.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM711_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM712_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000712</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP12</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP12</t>
-  </si>
-  <si>
-    <t>Edye presenta: Es Halloween y Norman está convencido de que va a ganar la competencia de asustar a todos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Es Halloween y todos en Pontypandy esperan con ansias la gran fiesta en casa de los Floods. Norman está convencido de que va a ganar la competencia de asustar a todos, pero Mandy confía en que ella saldrá victoriosa.</t>
-  </si>
-  <si>
-    <t>EEFSAM712.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM712_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM713_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000713</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP13</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP13</t>
-  </si>
-  <si>
-    <t>Edye presenta: Es el día libre de Sam y la estación está a cargo de Elvis y Penny, quien está resfriada.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Es el día libre de Sam y la estación está a cargo de Elvis y Penny, quien está resfriada. Mientras tanto, la familia Jones disfruta de la playa cuando ven a su gato en el techo del cobertizo. Llaman a la estación de bomberos para rescatarlo.</t>
-  </si>
-  <si>
-    <t>EEFSAM713.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM713_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM714_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000714</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP14</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP14</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los niños Norman, James, Mandy y Sarah juegan a ser piratas, pero una pelea los pone en riesgo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los niños de Pontypandy: Norman, James, Mandy y Sarah juegan a ser piratas, pero una pelea los divide en chicos y chicas. Los niños pirata se roban el almuerzo y se adentran al mar; la marea se los lleva y tienen que ser rescatados por Sam.</t>
-  </si>
-  <si>
-    <t>EEFSAM714.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM714_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM715_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000715</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP15</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP15</t>
-  </si>
-  <si>
-    <t>Edye presenta: Sam planea llevar de paseo a los niños de Pontypandy, pero lo llaman a revisar unas cajas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El bombero Sam planea un paseo de exploración con los niños Pioneros de Pontypandy, pero es llamado para revisar unas cajas en la playa. Norman ve la oportunidad de convertirse en líder de los Pioneros, hasta que Trevor interrumpe sus planes.</t>
-  </si>
-  <si>
-    <t>EEFSAM715.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM715_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM716_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000716</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP16</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP16</t>
-  </si>
-  <si>
-    <t>Edye presenta: Elvis es invitado a un programa de TV y sueña con cantar y convertirseen un estrella.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Un programa de TV invita a Elvis a cantar lo que lo hace soñar con convertirse en una superestrella del canto. Mientras tanto, Trevor y Norman van al bosque en busca de una rara ave llamada Curruca de cresta escarlata.</t>
-  </si>
-  <si>
-    <t>EEFSAM716.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM716_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM717_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000717</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP17</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP17</t>
-  </si>
-  <si>
-    <t>Edye presenta: El primo de Norman, Derek, llega a quedarse; Norman siente celos de él y lo aleja con engaños.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El primo de Norman, Derek, llega para quedarse, pero como es muy lindo y ordenado, Norman siente celos; planea su venganza, y lo envía a recoger unas flores inexistentes en la montaña. Arrepentido, le llama a Sam para que vaya a rescatarlo.</t>
-  </si>
-  <si>
-    <t>EEFSAM717.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM717_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM718_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000718</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP18</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP18</t>
-  </si>
-  <si>
-    <t>Edye presenta: El bombero Sam y el resto del equipo entrenan a Mike Flood y Charlie Jones para ser bomberos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Sam y el resto del equipo entrenan a Mike Flood y Charlie Jones para ser bomberos de reserva y el oficial Steele está contento con su progreso. Charlie y Mike están ansiosos por apagar su primer incendio pero Charlie también debe de salir de pesca.</t>
-  </si>
-  <si>
-    <t>EEFSAM718.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM718_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM719_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000719</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP19</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP19</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los bomberos Sam, Elvis y Penny hacen controles de rutina en diversos hidrantes de Pontypandy.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los bomberos Sam, Elvis y Penny hacen controles de rutina en algunos hidrantes alrededor de Pontypandy. Elvis está muy emocionado y convence a Sam para que lo deje usar la radio. Mientras, James y Sarah juegan a ser bomberos con sus walkie-talkie.</t>
-  </si>
-  <si>
-    <t>EEFSAM719.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM719_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM720_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000720</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP20</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP20</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman baja equipado para divertirse hasta que Bronwyn le ha dado a Dilys un regalo</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman baja de su habitación con un balón de futbol debajo de un brazo y una patineta en el otro, ansioso de salir al sol de Pontypandy y jugar con sus amigos. Antes de que pueda cruzar la puerta ve que Bronwyn le ha dado a Dilys un regalo.</t>
-  </si>
-  <si>
-    <t>EEFSAM720.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM720_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM721_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000721</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP21</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP21</t>
-  </si>
-  <si>
-    <t>Edye presenta: El jefe de estación, Steele, se toma el día libre para ir con Trevor y la pandilla a la costa.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El jefe de la estación, Norris Steele, se toma el día libre para ir con Trevor y la pandilla a la costa. Dilys ha preparado el almuerzo y junto con Mandy, Helen, Steele, Norman y Trevor suben al autobús. El jefe asegura haber trazado la mejor ruta.</t>
-  </si>
-  <si>
-    <t>EEFSAM721.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM721_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM722_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000722</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP22</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP22</t>
-  </si>
-  <si>
-    <t>Edye presenta: James tiene un nuevo avión de control remoto con el que él y Norman pueden jugar en el muelle.</t>
-  </si>
-  <si>
-    <t>Edye presenta: James tiene un nuevo avión de control remoto con el que Norman y él pueden jugar en el muelle. Norman está ansioso por ir, pero James se muestra reacio. Norman lo convence de que lo deje hacer maniobras con el avión y piensa que James es aburrido.</t>
-  </si>
-  <si>
-    <t>EEFSAM722.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM722_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM723_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000723</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP23</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP23</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman y Dilys practican para la carrera de tres patas de Pontypandy, pero Norman hace trampa.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman y Dilys practican para la carrera de tres patas de Pontypandy. Dilys no es muy buena en eso y Norman se siente harto; cree que tener a su madre de compañera no es buena idea y quiere a alguien más; para ganar hace trampa pero todo le sale mal.</t>
-  </si>
-  <si>
-    <t>EEFSAM723.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM723_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM724_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000724</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP24</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP24</t>
-  </si>
-  <si>
-    <t>Edye presenta: Norman se despierta una mañana y ve que todo Pontypandy está inundado. Sam inicia el rescate.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Una mañana, al despertar, Norman se da cuenta que todo Pontypandy está inundado. El bombero Sam va con Tom en su helicóptero para examinar la magnitud de la inundación. La familia Jones está varada en el techo de Wholefish Café. Sam los rescata.</t>
-  </si>
-  <si>
-    <t>EEFSAM724.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM724_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM725_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000725</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP25</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP25</t>
-  </si>
-  <si>
-    <t>Edye presenta: La estación de bomberos de Pontypandy está abierta al público y todos pueden ver lo que hacen.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Hoy en día la estación de bomberos de Pontypandy está abierta al público y todos pueden ver lo que hace un bombero cuando no está en emergencia. El oficial de la estación es el maestro de ceremonias y anuncia a todos lo que pasará en este lugar.</t>
-  </si>
-  <si>
-    <t>EEFSAM725.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM725_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM726_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS6000000000000726</t>
-  </si>
-  <si>
-    <t>Sam, El BomberoT07EP26</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP26</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mike practica para el gran lanzamiento de su cohete, pero Norman puede causar un accidente.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Mike practica para el gran lanzamiento de su cohete y espera presentárselos a todos en Pontypandy. Sin embargo, Sam y su equipo son llamados a una emergencia porque Norman ha lanzado su propio cohete, hecho sin calidad y puede causar un accidente.</t>
-  </si>
-  <si>
-    <t>EEFSAM726.mpg</t>
-  </si>
-  <si>
-    <t>EEFSAM726_land.jpg</t>
-  </si>
-  <si>
-    <t>EEFSAM701_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000701</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP01 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM701.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM702_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000702</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP02 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM702.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM703_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000703</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP03 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM703.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM704_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000704</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP04 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM704.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM705_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000705</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP05 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM705.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM706_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000706</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP06 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM706.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM707_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000707</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP07 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM707.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM708_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000708</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP08 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM708.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM709_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000709</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP09 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM709.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM710_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000710</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP10 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM710.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM711_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000711</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP11 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM711.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM712_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000712</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP12 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM712.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM713_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000713</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP13 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM713.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM714_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000714</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP14 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM714.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM715_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000715</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP15 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM715.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM716_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000716</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP16 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM716.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM717_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000717</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP17 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM717.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM718_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000718</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP18 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM718.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM719_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000719</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP19 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM719.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM720_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000720</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP20 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM720.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM721_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000721</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP21 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM721.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM722_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000722</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP22 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM722.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM723_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000723</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP23 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM723.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM724_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000724</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP24 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM724.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM725_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000725</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP25 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM725.ts</t>
-  </si>
-  <si>
-    <t>EEFSAM726_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEFS7000000000000726</t>
-  </si>
-  <si>
-    <t>Sam, El Bombero T07 EP26 HD</t>
-  </si>
-  <si>
-    <t>EEFSAM726.ts</t>
+    <t>EETDHM401_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000401</t>
+  </si>
+  <si>
+    <t>Serie El día que Henry conoció…</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP01</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP01</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un crucero con muchos pasajeros, pero ningún capitán. Henry se vuelve capitán.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un crucero y aprende lo que es un crucero. Crucero tiene una enorme fila de vacacionistas listos para abordar, pero su capitán está mareado. Henry se convierte en capitán de crucero y navega por todo el Caribe.</t>
+  </si>
+  <si>
+    <t>00:05:00</t>
+  </si>
+  <si>
+    <t>00:05</t>
+  </si>
+  <si>
+    <t>Infantil/El día que Henry conoció…</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Darragh Malone, Oliver Callan, Lisa Garvey, Daniel O'Gorman, Chloe Corbett, Gilly Breen Moya, Henry Gill, Scarlett Solórzano, Emily Corbett, Ben Corbett, Finan Breen, Joe Hyland, Fia Brennan, Breen, Joann.</t>
+  </si>
+  <si>
+    <t>Wiggleywoo</t>
+  </si>
+  <si>
+    <t>Malone Darragh, Callan Oliver, Garvey Lisa, O'Gorman Daniel, Corbett Chloe, Moya Gilly Breen, Gill Henry, Solórzano Scarlett, Corbett Emily, Corbett Ben, Breen Finan, Hyland Joe, Brennan Fia, Breen, Joann.</t>
+  </si>
+  <si>
+    <t>Moya, Gilly Breen</t>
+  </si>
+  <si>
+    <t>EETDHM401.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM4_box.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM401_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM402_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000402</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP02</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP02</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un Algodón de Azúcar en la feria. Pero todos los operarios están enfermos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un Algodón de Azúcar en la feria. Todos los trabajadores de la feria están enfermos, así que nadie puede manejar los juegos. ¡Tendrán que cerrar! Henry se convierte en trabajador de la feria y tiene que operar todas las atracciones.</t>
+  </si>
+  <si>
+    <t>EETDHM402.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM402_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM403_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000403</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP03</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP03</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una botella de leche. Al no haber quien las reparta, Henry se vuelve lechero.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una botella de leche en su escalón. Henry aprende todo sobre los beneficios de tomar leche y de dónde viene. Henry se convierte en lechero, viaja en su camioneta de reparto y entrega leche a tiempo para el desayuno de todos.</t>
+  </si>
+  <si>
+    <t>EETDHM403.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM403_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM404_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000404</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP04</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP04</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una motocicleta que sueña con saltar el Gran Cañón. Henry se hace motociclista.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una motocicleta que siempre quiso saltar el Gran Cañón. Henry se convierte en motociclista acrobático y la ayuda a cumplir su sueño.</t>
+  </si>
+  <si>
+    <t>EETDHM404.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM404_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM405_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000405</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP05</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP05</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una linterna que siempre quiso explorar una vieja casa embrujada.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una linterna que siempre quiso explorar una vieja casa embrujada. Henry se convierte en investigador paranormal y ayuda a Linterna a explorar la Vieja Casa Embrujada.</t>
+  </si>
+  <si>
+    <t>EETDHM405.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM405_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM406_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000406</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP06</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP06</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce una rosa en el día de los enamorados. Pero el florista está enfermo.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una rosa. Henry aprende sobre el Día de San Valentín y lo que hace una florista. Desafortunadamente el florista tiene fiebre del heno, así que no hay nadie para armar los ramos. Henry se convierte en florista y ayuda a hacerlos.</t>
+  </si>
+  <si>
+    <t>EETDHM406.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM406_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM407_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000407</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP07</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP07</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un taxi que no tiene chofer. Henry se convierte en taxista de Nueva York.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry se convierte en un taxista de Nueva York, y aprende para qué se usan los taxis, qué es la Gan Manzana y ve los diferentes paisajes de Nueva York. Henry se convierte en taxista de Nueva York y sale a buscar pasajeros.</t>
+  </si>
+  <si>
+    <t>EETDHM407.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM407_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM408_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000408</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP08</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP08</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una tabla de nieve que nunca ha salido de la tienda de deportes extremos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una tabla de nieve en una tienda de deportes extremos. Lo aprende todo sobre los deportes de montaña. Pero la tabla nunca ha salido de la tienda. Henry se convierte en snowboarder y viaja a la base de una hermosa montaña nevada.</t>
+  </si>
+  <si>
+    <t>EETDHM408.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM408_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM409_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000409</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP09</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP09</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una vieja góndola que nunca transportó a turistas de paseo por Venecia.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una vieja góndola en un astillero desvencijado, y lo aprende todo sobre los botes y como se han usado para el transporte durante cientos de años. Henry se convierte en gondolero y comienza a transportar turistas por Venecia.</t>
+  </si>
+  <si>
+    <t>EETDHM409.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM409_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM410_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000410</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP10</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP10</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una hormiga encerrada en una granja de hormigas que quiere regresar a su nido.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una hormiga que está encerrada en una granja de hormigas, La hormiga quiere regresar a su nido en el jardín y Henry se convierte en hormiga para ayudarla.</t>
+  </si>
+  <si>
+    <t>EETDHM410.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM410_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM411_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000411</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP11</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP11</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a patines sobre hielo que desean participar a un evento de patinaje artístico.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un par de patines sobre hielo que desean participar a un espectáculo de patinaje artístico. Al no haber un patinador, Henry se convierte en uno para ayudarlos a cumplir su sueño.</t>
+  </si>
+  <si>
+    <t>EETDHM411.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM411_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM412_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000412</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP12</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP12</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una motoneta de pizzería en Roma. Pero no hay nadie que las prepare y reparta.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a una motoneta en la capital de Italia, Roma, y reparte pizza. Henry lo aprende todo sobre hacer pizza y se convierte en motociclista repartidor de pizza.</t>
+  </si>
+  <si>
+    <t>EETDHM412.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM412_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM413_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000413</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP13</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP13</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un paracaídas que quiere dar el mayor salto mundial. Pero falta un paracaidista.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un paracaídas, y lo aprende todo sobre el paracaidismo, los paracaídas y cómo funcionan. Paracaídas quiere hacer el salto más alto del mundo. Henry se convierte en paracaidista y lo ayuda a dar el salto más alto del mundo.</t>
+  </si>
+  <si>
+    <t>EETDHM413.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM413_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM414_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000414</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP14</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP14</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un cangrejo ermitaño que busca un nuevo hogar en una playa muy contaminada.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un cangrejo ermitaño y aprende sobre la contaminación y cómo algunas personas arrojan basura por todas partes de la playa. Henry se convierte en ambientalista y ayuda a limpiar.</t>
+  </si>
+  <si>
+    <t>EETDHM414.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM414_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM415_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000415</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP15</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP15</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce una caja de herramientas que quiere fabricar invenciones. Pero no hay carpintero.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una caja de herramientas y aprende sobre el trabajo de un carpintero. Henry se convierte en carpintero y ayuda a hacer todo tipo de trabajos con la caja.</t>
+  </si>
+  <si>
+    <t>EETDHM415.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM415_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM416_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000416</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP16</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP16</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un husky que necesita de un explorador del ártico para emprender su viaje.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un husky y aprende sobre el trabajo de estos perros. Henry aprende que los huskys tiran de trineos por la nieve. Henry se convierte en un gran explorador del ártico y viaja al Ártico con Husky.</t>
+  </si>
+  <si>
+    <t>EETDHM416.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM416_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM417_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000417</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP17</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP17</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una corona que quiere hacer un banquete medieval pero falta le falta un bufón.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a una corona y aprende sobre los objetos reales. Corona quiere hacer un banquete medieval y Henry se convierte en bufón de la corte y entretiene a los comensales.</t>
+  </si>
+  <si>
+    <t>EETDHM417.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM417_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM418_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000418</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP18</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP18</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce un folleto en un museo que promueve la nueva gran exhibición. Pero falta el guía.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce un folleto de museo. Hay muchos turistas esperando afuera, pero el guía no está. Henry se convierte en guía y le muestra a los visitantes las riquezas contenidas en el museo.</t>
+  </si>
+  <si>
+    <t>EETDHM418.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM418_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM419_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000419</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP19</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP19</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un saxófono que quiere tocar jazz con su banda en la Nueva Orleans.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un saxófono tocando en la calle en Dublín. Henry aprende todo sobre los músicos callejeros y la música que tocan. Henry se convierte en cantante de jazz y toca en Nueva Orleans con el Saxófono.</t>
+  </si>
+  <si>
+    <t>EETDHM419.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM419_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM420_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000420</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP20</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP20</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un carruaje que sueña con participar en una carrera en la antigua Roma.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un carruaje que vive en una excavación arqueológica y se convierte en conductor para participar en una carrera en la antigua Roma. </t>
+  </si>
+  <si>
+    <t>EETDHM420.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM420_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM421_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000421</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP21</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP21</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un balde y un trapeador que trabajan en el acuario que no abre: falta un pez.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un balde y un trapeador que trabajan en el acuario dejando los pisos impecables. Henry aprende sobre la vida marina y se convierte en acuarista.</t>
+  </si>
+  <si>
+    <t>EETDHM421.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM421_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM422_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000422</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP22</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP22</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un rodillo de pintura listo para decorar una casa. Pero falta la mano de obra.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un Rodillo de Pintura y aprende a decorar. Henry se convierte en pintor decorador y ayuda a decorar la casa para los nuevos dueños.</t>
+  </si>
+  <si>
+    <t>EETDHM422.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM422_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM423_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000423</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP23</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP23</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a un laúd que necesita un aventurero para poder volver a cantar sus hazañas.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a un laúd que canta y narra todo lo que sucede en el episodio. El laúd no ha vivido una aventura excitante para cantar desde hace tiempo, y necesita de un intrépido aventurero para poder volver a hacerlo. Henry se hace aventurero.</t>
+  </si>
+  <si>
+    <t>EETDHM423.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM423_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM424_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000424</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP24</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP24</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una tarjeta de biblioteca que quiere revivir grandes eventos históricos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Henry conoce a una tarjeta de biblioteca y lo aprende todo sobre libros y bibliotecas. Los libros favoritos de la tarjeta son los de historia. Henry y Tarjeta se hacen viajeros del tiempo y viajan al pasado para experimentar eventos históricos.</t>
+  </si>
+  <si>
+    <t>EETDHM424.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM424_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM425_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000425</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP25</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP25</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a una boa de plumas que sospecha de las otras prendas de vestir.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce a una boa de plumas que teme que las otras prendas estén actuando sospechosamente. Henry se convierte en investigador privado y trata de resolver el misterio de las prendas sospechosas.</t>
+  </si>
+  <si>
+    <t>EETDHM425.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM425_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM426_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD6000000000000426</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció…T04EP26</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP26</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una batisfera de utilería que quiere explorar el fondo de los océanos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hoy Henry conoce una batisfera y aprende que es un vehículo muy especial de las profundidades y lleva a los pasajeros al fondo del océano. Henry se convierte en biólogo marino y viaja al fondo del mar.</t>
+  </si>
+  <si>
+    <t>00:04:59</t>
+  </si>
+  <si>
+    <t>EETDHM426.mpg</t>
+  </si>
+  <si>
+    <t>EETDHM426_land.jpg</t>
+  </si>
+  <si>
+    <t>EETDHM401_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000401</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP01 HD</t>
+  </si>
+  <si>
+    <t>EETDHM401.ts</t>
+  </si>
+  <si>
+    <t>EETDHM402_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000402</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP02 HD</t>
+  </si>
+  <si>
+    <t>EETDHM402.ts</t>
+  </si>
+  <si>
+    <t>EETDHM403_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000403</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP03 HD</t>
+  </si>
+  <si>
+    <t>EETDHM403.ts</t>
+  </si>
+  <si>
+    <t>EETDHM404_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000404</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP04 HD</t>
+  </si>
+  <si>
+    <t>EETDHM404.ts</t>
+  </si>
+  <si>
+    <t>EETDHM405_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000405</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP05 HD</t>
+  </si>
+  <si>
+    <t>EETDHM405.ts</t>
+  </si>
+  <si>
+    <t>EETDHM406_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000406</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP06 HD</t>
+  </si>
+  <si>
+    <t>EETDHM406.ts</t>
+  </si>
+  <si>
+    <t>EETDHM407_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000407</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP07 HD</t>
+  </si>
+  <si>
+    <t>EETDHM407.ts</t>
+  </si>
+  <si>
+    <t>EETDHM408_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000408</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP08 HD</t>
+  </si>
+  <si>
+    <t>EETDHM408.ts</t>
+  </si>
+  <si>
+    <t>EETDHM409_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000409</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP09 HD</t>
+  </si>
+  <si>
+    <t>EETDHM409.ts</t>
+  </si>
+  <si>
+    <t>EETDHM410_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000410</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP10 HD</t>
+  </si>
+  <si>
+    <t>EETDHM410.ts</t>
+  </si>
+  <si>
+    <t>EETDHM411_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000411</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP11 HD</t>
+  </si>
+  <si>
+    <t>EETDHM411.ts</t>
+  </si>
+  <si>
+    <t>EETDHM412_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000412</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP12 HD</t>
+  </si>
+  <si>
+    <t>EETDHM412.ts</t>
+  </si>
+  <si>
+    <t>EETDHM413_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000413</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP13 HD</t>
+  </si>
+  <si>
+    <t>EETDHM413.ts</t>
+  </si>
+  <si>
+    <t>EETDHM414_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000414</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP14 HD</t>
+  </si>
+  <si>
+    <t>EETDHM414.ts</t>
+  </si>
+  <si>
+    <t>EETDHM415_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000415</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP15 HD</t>
+  </si>
+  <si>
+    <t>EETDHM415.ts</t>
+  </si>
+  <si>
+    <t>EETDHM416_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000416</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP16 HD</t>
+  </si>
+  <si>
+    <t>EETDHM416.ts</t>
+  </si>
+  <si>
+    <t>EETDHM417_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000417</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP17 HD</t>
+  </si>
+  <si>
+    <t>EETDHM417.ts</t>
+  </si>
+  <si>
+    <t>EETDHM418_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000418</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP18 HD</t>
+  </si>
+  <si>
+    <t>EETDHM418.ts</t>
+  </si>
+  <si>
+    <t>EETDHM419_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000419</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP19 HD</t>
+  </si>
+  <si>
+    <t>EETDHM419.ts</t>
+  </si>
+  <si>
+    <t>EETDHM420_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000420</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP20 HD</t>
+  </si>
+  <si>
+    <t>EETDHM420.ts</t>
+  </si>
+  <si>
+    <t>EETDHM421_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000421</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP21 HD</t>
+  </si>
+  <si>
+    <t>EETDHM421.ts</t>
+  </si>
+  <si>
+    <t>EETDHM422_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000422</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP22 HD</t>
+  </si>
+  <si>
+    <t>EETDHM422.ts</t>
+  </si>
+  <si>
+    <t>EETDHM423_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000423</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP23 HD</t>
+  </si>
+  <si>
+    <t>EETDHM423.ts</t>
+  </si>
+  <si>
+    <t>EETDHM424_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000424</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP24 HD</t>
+  </si>
+  <si>
+    <t>EETDHM424.ts</t>
+  </si>
+  <si>
+    <t>EETDHM425_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000425</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP25 HD</t>
+  </si>
+  <si>
+    <t>EETDHM425.ts</t>
+  </si>
+  <si>
+    <t>EETDHM426_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EETD7000000000000426</t>
+  </si>
+  <si>
+    <t>El día que Henry conoció… T04 EP26 HD</t>
+  </si>
+  <si>
+    <t>EETDHM426.ts</t>
   </si>
 </sst>
 </file>
@@ -7586,7 +7589,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:BF58"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:BF58"/>
     </sheetView>
   </sheetViews>
@@ -7770,7 +7773,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -7828,7 +7831,7 @@
         <v>99</v>
       </c>
       <c r="V2" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>100</v>
@@ -7840,10 +7843,10 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA2" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>49</v>
@@ -7895,7 +7898,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>55</v>
@@ -7938,7 +7941,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>43</v>
@@ -7996,7 +7999,7 @@
         <v>99</v>
       </c>
       <c r="V3" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>100</v>
@@ -8008,10 +8011,10 @@
         <v>44</v>
       </c>
       <c r="Z3" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA3" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB3" s="6" t="s">
         <v>49</v>
@@ -8063,7 +8066,7 @@
         <v>54</v>
       </c>
       <c r="AS3" s="6">
-        <v>281936080</v>
+        <v>141297980</v>
       </c>
       <c r="AT3" s="6" t="s">
         <v>55</v>
@@ -8106,7 +8109,7 @@
         <v>118</v>
       </c>
       <c r="B4" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>43</v>
@@ -8164,7 +8167,7 @@
         <v>99</v>
       </c>
       <c r="V4" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>100</v>
@@ -8176,10 +8179,10 @@
         <v>44</v>
       </c>
       <c r="Z4" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA4" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB4" s="6" t="s">
         <v>49</v>
@@ -8231,7 +8234,7 @@
         <v>54</v>
       </c>
       <c r="AS4" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT4" s="6" t="s">
         <v>55</v>
@@ -8274,7 +8277,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>43</v>
@@ -8332,7 +8335,7 @@
         <v>99</v>
       </c>
       <c r="V5" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>100</v>
@@ -8344,10 +8347,10 @@
         <v>44</v>
       </c>
       <c r="Z5" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA5" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>49</v>
@@ -8399,7 +8402,7 @@
         <v>54</v>
       </c>
       <c r="AS5" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT5" s="6" t="s">
         <v>55</v>
@@ -8442,7 +8445,7 @@
         <v>134</v>
       </c>
       <c r="B6" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>43</v>
@@ -8500,7 +8503,7 @@
         <v>99</v>
       </c>
       <c r="V6" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>100</v>
@@ -8512,10 +8515,10 @@
         <v>44</v>
       </c>
       <c r="Z6" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA6" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>49</v>
@@ -8567,7 +8570,7 @@
         <v>54</v>
       </c>
       <c r="AS6" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT6" s="6" t="s">
         <v>55</v>
@@ -8610,7 +8613,7 @@
         <v>142</v>
       </c>
       <c r="B7" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -8668,7 +8671,7 @@
         <v>99</v>
       </c>
       <c r="V7" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>100</v>
@@ -8680,10 +8683,10 @@
         <v>44</v>
       </c>
       <c r="Z7" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA7" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>49</v>
@@ -8735,7 +8738,7 @@
         <v>54</v>
       </c>
       <c r="AS7" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT7" s="6" t="s">
         <v>55</v>
@@ -8778,7 +8781,7 @@
         <v>150</v>
       </c>
       <c r="B8" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>43</v>
@@ -8836,7 +8839,7 @@
         <v>99</v>
       </c>
       <c r="V8" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>100</v>
@@ -8848,10 +8851,10 @@
         <v>44</v>
       </c>
       <c r="Z8" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA8" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB8" s="6" t="s">
         <v>49</v>
@@ -8903,7 +8906,7 @@
         <v>54</v>
       </c>
       <c r="AS8" s="6">
-        <v>281456868</v>
+        <v>141297980</v>
       </c>
       <c r="AT8" s="6" t="s">
         <v>55</v>
@@ -8946,7 +8949,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>43</v>
@@ -9004,7 +9007,7 @@
         <v>99</v>
       </c>
       <c r="V9" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W9" s="6" t="s">
         <v>100</v>
@@ -9016,10 +9019,10 @@
         <v>44</v>
       </c>
       <c r="Z9" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA9" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB9" s="6" t="s">
         <v>49</v>
@@ -9071,7 +9074,7 @@
         <v>54</v>
       </c>
       <c r="AS9" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT9" s="6" t="s">
         <v>55</v>
@@ -9114,7 +9117,7 @@
         <v>166</v>
       </c>
       <c r="B10" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
@@ -9172,7 +9175,7 @@
         <v>99</v>
       </c>
       <c r="V10" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W10" s="6" t="s">
         <v>100</v>
@@ -9184,10 +9187,10 @@
         <v>44</v>
       </c>
       <c r="Z10" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA10" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB10" s="6" t="s">
         <v>49</v>
@@ -9239,7 +9242,7 @@
         <v>54</v>
       </c>
       <c r="AS10" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT10" s="6" t="s">
         <v>55</v>
@@ -9282,7 +9285,7 @@
         <v>174</v>
       </c>
       <c r="B11" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>43</v>
@@ -9340,7 +9343,7 @@
         <v>99</v>
       </c>
       <c r="V11" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W11" s="6" t="s">
         <v>100</v>
@@ -9352,10 +9355,10 @@
         <v>44</v>
       </c>
       <c r="Z11" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA11" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB11" s="6" t="s">
         <v>49</v>
@@ -9407,7 +9410,7 @@
         <v>54</v>
       </c>
       <c r="AS11" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT11" s="6" t="s">
         <v>55</v>
@@ -9450,7 +9453,7 @@
         <v>182</v>
       </c>
       <c r="B12" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>43</v>
@@ -9508,7 +9511,7 @@
         <v>99</v>
       </c>
       <c r="V12" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W12" s="6" t="s">
         <v>100</v>
@@ -9520,10 +9523,10 @@
         <v>44</v>
       </c>
       <c r="Z12" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA12" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB12" s="6" t="s">
         <v>49</v>
@@ -9575,7 +9578,7 @@
         <v>54</v>
       </c>
       <c r="AS12" s="6">
-        <v>281907316</v>
+        <v>141297980</v>
       </c>
       <c r="AT12" s="6" t="s">
         <v>55</v>
@@ -9618,7 +9621,7 @@
         <v>190</v>
       </c>
       <c r="B13" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>43</v>
@@ -9676,7 +9679,7 @@
         <v>99</v>
       </c>
       <c r="V13" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W13" s="6" t="s">
         <v>100</v>
@@ -9688,10 +9691,10 @@
         <v>44</v>
       </c>
       <c r="Z13" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA13" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>49</v>
@@ -9743,7 +9746,7 @@
         <v>54</v>
       </c>
       <c r="AS13" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT13" s="6" t="s">
         <v>55</v>
@@ -9786,7 +9789,7 @@
         <v>198</v>
       </c>
       <c r="B14" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>43</v>
@@ -9844,7 +9847,7 @@
         <v>99</v>
       </c>
       <c r="V14" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W14" s="6" t="s">
         <v>100</v>
@@ -9856,10 +9859,10 @@
         <v>44</v>
       </c>
       <c r="Z14" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA14" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB14" s="6" t="s">
         <v>49</v>
@@ -9911,7 +9914,7 @@
         <v>54</v>
       </c>
       <c r="AS14" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT14" s="6" t="s">
         <v>55</v>
@@ -9954,7 +9957,7 @@
         <v>206</v>
       </c>
       <c r="B15" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>43</v>
@@ -10012,7 +10015,7 @@
         <v>99</v>
       </c>
       <c r="V15" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W15" s="6" t="s">
         <v>100</v>
@@ -10024,10 +10027,10 @@
         <v>44</v>
       </c>
       <c r="Z15" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA15" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB15" s="6" t="s">
         <v>49</v>
@@ -10079,7 +10082,7 @@
         <v>54</v>
       </c>
       <c r="AS15" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT15" s="6" t="s">
         <v>55</v>
@@ -10122,7 +10125,7 @@
         <v>214</v>
       </c>
       <c r="B16" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>43</v>
@@ -10180,7 +10183,7 @@
         <v>99</v>
       </c>
       <c r="V16" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W16" s="6" t="s">
         <v>100</v>
@@ -10192,10 +10195,10 @@
         <v>44</v>
       </c>
       <c r="Z16" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA16" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB16" s="6" t="s">
         <v>49</v>
@@ -10247,7 +10250,7 @@
         <v>54</v>
       </c>
       <c r="AS16" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT16" s="6" t="s">
         <v>55</v>
@@ -10290,7 +10293,7 @@
         <v>222</v>
       </c>
       <c r="B17" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>43</v>
@@ -10348,7 +10351,7 @@
         <v>99</v>
       </c>
       <c r="V17" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W17" s="6" t="s">
         <v>100</v>
@@ -10360,10 +10363,10 @@
         <v>44</v>
       </c>
       <c r="Z17" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA17" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB17" s="6" t="s">
         <v>49</v>
@@ -10415,7 +10418,7 @@
         <v>54</v>
       </c>
       <c r="AS17" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT17" s="6" t="s">
         <v>55</v>
@@ -10458,7 +10461,7 @@
         <v>230</v>
       </c>
       <c r="B18" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>43</v>
@@ -10516,7 +10519,7 @@
         <v>99</v>
       </c>
       <c r="V18" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W18" s="6" t="s">
         <v>100</v>
@@ -10528,10 +10531,10 @@
         <v>44</v>
       </c>
       <c r="Z18" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA18" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB18" s="6" t="s">
         <v>49</v>
@@ -10583,7 +10586,7 @@
         <v>54</v>
       </c>
       <c r="AS18" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT18" s="6" t="s">
         <v>55</v>
@@ -10626,7 +10629,7 @@
         <v>238</v>
       </c>
       <c r="B19" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>43</v>
@@ -10684,7 +10687,7 @@
         <v>99</v>
       </c>
       <c r="V19" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W19" s="6" t="s">
         <v>100</v>
@@ -10696,10 +10699,10 @@
         <v>44</v>
       </c>
       <c r="Z19" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA19" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB19" s="6" t="s">
         <v>49</v>
@@ -10751,7 +10754,7 @@
         <v>54</v>
       </c>
       <c r="AS19" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT19" s="6" t="s">
         <v>55</v>
@@ -10794,7 +10797,7 @@
         <v>246</v>
       </c>
       <c r="B20" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>43</v>
@@ -10852,7 +10855,7 @@
         <v>99</v>
       </c>
       <c r="V20" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W20" s="6" t="s">
         <v>100</v>
@@ -10864,10 +10867,10 @@
         <v>44</v>
       </c>
       <c r="Z20" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA20" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB20" s="6" t="s">
         <v>49</v>
@@ -10919,7 +10922,7 @@
         <v>54</v>
       </c>
       <c r="AS20" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT20" s="6" t="s">
         <v>55</v>
@@ -10962,7 +10965,7 @@
         <v>254</v>
       </c>
       <c r="B21" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>43</v>
@@ -11020,7 +11023,7 @@
         <v>99</v>
       </c>
       <c r="V21" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W21" s="6" t="s">
         <v>100</v>
@@ -11032,10 +11035,10 @@
         <v>44</v>
       </c>
       <c r="Z21" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA21" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB21" s="6" t="s">
         <v>49</v>
@@ -11087,7 +11090,7 @@
         <v>54</v>
       </c>
       <c r="AS21" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT21" s="6" t="s">
         <v>55</v>
@@ -11130,7 +11133,7 @@
         <v>262</v>
       </c>
       <c r="B22" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>43</v>
@@ -11188,7 +11191,7 @@
         <v>99</v>
       </c>
       <c r="V22" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W22" s="6" t="s">
         <v>100</v>
@@ -11200,10 +11203,10 @@
         <v>44</v>
       </c>
       <c r="Z22" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA22" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB22" s="6" t="s">
         <v>49</v>
@@ -11255,7 +11258,7 @@
         <v>54</v>
       </c>
       <c r="AS22" s="6">
-        <v>281907316</v>
+        <v>141252108</v>
       </c>
       <c r="AT22" s="6" t="s">
         <v>55</v>
@@ -11298,7 +11301,7 @@
         <v>270</v>
       </c>
       <c r="B23" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>43</v>
@@ -11356,7 +11359,7 @@
         <v>99</v>
       </c>
       <c r="V23" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W23" s="6" t="s">
         <v>100</v>
@@ -11368,10 +11371,10 @@
         <v>44</v>
       </c>
       <c r="Z23" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA23" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB23" s="6" t="s">
         <v>49</v>
@@ -11423,7 +11426,7 @@
         <v>54</v>
       </c>
       <c r="AS23" s="6">
-        <v>281907316</v>
+        <v>141206236</v>
       </c>
       <c r="AT23" s="6" t="s">
         <v>55</v>
@@ -11466,7 +11469,7 @@
         <v>278</v>
       </c>
       <c r="B24" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>43</v>
@@ -11524,7 +11527,7 @@
         <v>99</v>
       </c>
       <c r="V24" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W24" s="6" t="s">
         <v>100</v>
@@ -11536,10 +11539,10 @@
         <v>44</v>
       </c>
       <c r="Z24" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA24" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB24" s="6" t="s">
         <v>49</v>
@@ -11591,7 +11594,7 @@
         <v>54</v>
       </c>
       <c r="AS24" s="6">
-        <v>281893028</v>
+        <v>141206236</v>
       </c>
       <c r="AT24" s="6" t="s">
         <v>55</v>
@@ -11634,7 +11637,7 @@
         <v>286</v>
       </c>
       <c r="B25" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>43</v>
@@ -11692,7 +11695,7 @@
         <v>99</v>
       </c>
       <c r="V25" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W25" s="6" t="s">
         <v>100</v>
@@ -11704,10 +11707,10 @@
         <v>44</v>
       </c>
       <c r="Z25" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA25" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB25" s="6" t="s">
         <v>49</v>
@@ -11759,7 +11762,7 @@
         <v>54</v>
       </c>
       <c r="AS25" s="6">
-        <v>281907316</v>
+        <v>141266584</v>
       </c>
       <c r="AT25" s="6" t="s">
         <v>55</v>
@@ -11802,7 +11805,7 @@
         <v>294</v>
       </c>
       <c r="B26" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>43</v>
@@ -11860,7 +11863,7 @@
         <v>99</v>
       </c>
       <c r="V26" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W26" s="6" t="s">
         <v>100</v>
@@ -11872,10 +11875,10 @@
         <v>44</v>
       </c>
       <c r="Z26" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA26" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB26" s="6" t="s">
         <v>49</v>
@@ -11927,7 +11930,7 @@
         <v>54</v>
       </c>
       <c r="AS26" s="6">
-        <v>281907316</v>
+        <v>141280872</v>
       </c>
       <c r="AT26" s="6" t="s">
         <v>55</v>
@@ -11970,7 +11973,7 @@
         <v>302</v>
       </c>
       <c r="B27" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>43</v>
@@ -12022,13 +12025,13 @@
         <v>64</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>98</v>
+        <v>308</v>
       </c>
       <c r="U27" s="5" t="s">
         <v>99</v>
       </c>
       <c r="V27" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W27" s="6" t="s">
         <v>100</v>
@@ -12040,10 +12043,10 @@
         <v>44</v>
       </c>
       <c r="Z27" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA27" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB27" s="6" t="s">
         <v>49</v>
@@ -12095,7 +12098,7 @@
         <v>54</v>
       </c>
       <c r="AS27" s="6">
-        <v>281907316</v>
+        <v>140982516</v>
       </c>
       <c r="AT27" s="6" t="s">
         <v>55</v>
@@ -12104,7 +12107,7 @@
         <v>56</v>
       </c>
       <c r="AV27" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AW27" s="6"/>
       <c r="AX27" s="6" t="s">
@@ -12130,7 +12133,7 @@
         <v>60</v>
       </c>
       <c r="BF27" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.25">
@@ -16109,7 +16112,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:BF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:BF58"/>
     </sheetView>
   </sheetViews>
@@ -16290,10 +16293,10 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B2" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -16314,7 +16317,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>93</v>
@@ -16330,7 +16333,7 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>65</v>
@@ -16351,7 +16354,7 @@
         <v>99</v>
       </c>
       <c r="V2" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>100</v>
@@ -16363,10 +16366,10 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA2" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>49</v>
@@ -16418,7 +16421,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>54</v>
@@ -16427,7 +16430,7 @@
         <v>62</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AW2" s="6"/>
       <c r="AX2" s="6" t="s">
@@ -16458,10 +16461,10 @@
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B3" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>43</v>
@@ -16482,7 +16485,7 @@
         <v>46</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>93</v>
@@ -16498,7 +16501,7 @@
         <v>47</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>66</v>
@@ -16519,7 +16522,7 @@
         <v>99</v>
       </c>
       <c r="V3" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>100</v>
@@ -16531,10 +16534,10 @@
         <v>44</v>
       </c>
       <c r="Z3" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA3" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB3" s="6" t="s">
         <v>49</v>
@@ -16586,7 +16589,7 @@
         <v>54</v>
       </c>
       <c r="AS3" s="6">
-        <v>563814444</v>
+        <v>282532792</v>
       </c>
       <c r="AT3" s="6" t="s">
         <v>54</v>
@@ -16595,7 +16598,7 @@
         <v>62</v>
       </c>
       <c r="AV3" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AW3" s="6"/>
       <c r="AX3" s="6" t="s">
@@ -16626,10 +16629,10 @@
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B4" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>43</v>
@@ -16650,7 +16653,7 @@
         <v>46</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>93</v>
@@ -16666,7 +16669,7 @@
         <v>47</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>67</v>
@@ -16687,7 +16690,7 @@
         <v>99</v>
       </c>
       <c r="V4" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>100</v>
@@ -16699,10 +16702,10 @@
         <v>44</v>
       </c>
       <c r="Z4" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA4" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB4" s="6" t="s">
         <v>49</v>
@@ -16754,7 +16757,7 @@
         <v>54</v>
       </c>
       <c r="AS4" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT4" s="6" t="s">
         <v>54</v>
@@ -16763,7 +16766,7 @@
         <v>62</v>
       </c>
       <c r="AV4" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AW4" s="6"/>
       <c r="AX4" s="6" t="s">
@@ -16794,10 +16797,10 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B5" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>43</v>
@@ -16818,7 +16821,7 @@
         <v>46</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>93</v>
@@ -16834,7 +16837,7 @@
         <v>47</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>68</v>
@@ -16855,7 +16858,7 @@
         <v>99</v>
       </c>
       <c r="V5" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>100</v>
@@ -16867,10 +16870,10 @@
         <v>44</v>
       </c>
       <c r="Z5" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA5" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>49</v>
@@ -16922,7 +16925,7 @@
         <v>54</v>
       </c>
       <c r="AS5" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT5" s="6" t="s">
         <v>54</v>
@@ -16931,7 +16934,7 @@
         <v>62</v>
       </c>
       <c r="AV5" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AW5" s="6"/>
       <c r="AX5" s="6" t="s">
@@ -16962,10 +16965,10 @@
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B6" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>43</v>
@@ -16986,7 +16989,7 @@
         <v>46</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>93</v>
@@ -17002,7 +17005,7 @@
         <v>47</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>69</v>
@@ -17023,7 +17026,7 @@
         <v>99</v>
       </c>
       <c r="V6" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>100</v>
@@ -17035,10 +17038,10 @@
         <v>44</v>
       </c>
       <c r="Z6" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA6" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>49</v>
@@ -17090,7 +17093,7 @@
         <v>54</v>
       </c>
       <c r="AS6" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT6" s="6" t="s">
         <v>54</v>
@@ -17099,7 +17102,7 @@
         <v>62</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AW6" s="6"/>
       <c r="AX6" s="6" t="s">
@@ -17130,10 +17133,10 @@
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B7" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -17154,7 +17157,7 @@
         <v>46</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>93</v>
@@ -17170,7 +17173,7 @@
         <v>47</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>70</v>
@@ -17191,7 +17194,7 @@
         <v>99</v>
       </c>
       <c r="V7" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>100</v>
@@ -17203,10 +17206,10 @@
         <v>44</v>
       </c>
       <c r="Z7" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA7" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>49</v>
@@ -17258,7 +17261,7 @@
         <v>54</v>
       </c>
       <c r="AS7" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT7" s="6" t="s">
         <v>54</v>
@@ -17267,7 +17270,7 @@
         <v>62</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AW7" s="6"/>
       <c r="AX7" s="6" t="s">
@@ -17298,10 +17301,10 @@
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B8" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>43</v>
@@ -17322,7 +17325,7 @@
         <v>46</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>93</v>
@@ -17338,7 +17341,7 @@
         <v>47</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>71</v>
@@ -17359,7 +17362,7 @@
         <v>99</v>
       </c>
       <c r="V8" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>100</v>
@@ -17371,10 +17374,10 @@
         <v>44</v>
       </c>
       <c r="Z8" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA8" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB8" s="6" t="s">
         <v>49</v>
@@ -17426,7 +17429,7 @@
         <v>54</v>
       </c>
       <c r="AS8" s="6">
-        <v>562856208</v>
+        <v>282532792</v>
       </c>
       <c r="AT8" s="6" t="s">
         <v>54</v>
@@ -17435,7 +17438,7 @@
         <v>62</v>
       </c>
       <c r="AV8" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AW8" s="6"/>
       <c r="AX8" s="6" t="s">
@@ -17466,10 +17469,10 @@
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B9" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>43</v>
@@ -17490,7 +17493,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>93</v>
@@ -17506,7 +17509,7 @@
         <v>47</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>72</v>
@@ -17527,7 +17530,7 @@
         <v>99</v>
       </c>
       <c r="V9" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W9" s="6" t="s">
         <v>100</v>
@@ -17539,10 +17542,10 @@
         <v>44</v>
       </c>
       <c r="Z9" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA9" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB9" s="6" t="s">
         <v>49</v>
@@ -17594,7 +17597,7 @@
         <v>54</v>
       </c>
       <c r="AS9" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT9" s="6" t="s">
         <v>54</v>
@@ -17603,7 +17606,7 @@
         <v>62</v>
       </c>
       <c r="AV9" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AW9" s="6"/>
       <c r="AX9" s="6" t="s">
@@ -17634,10 +17637,10 @@
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B10" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
@@ -17658,7 +17661,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>93</v>
@@ -17674,7 +17677,7 @@
         <v>47</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>73</v>
@@ -17695,7 +17698,7 @@
         <v>99</v>
       </c>
       <c r="V10" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W10" s="6" t="s">
         <v>100</v>
@@ -17707,10 +17710,10 @@
         <v>44</v>
       </c>
       <c r="Z10" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA10" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB10" s="6" t="s">
         <v>49</v>
@@ -17762,7 +17765,7 @@
         <v>54</v>
       </c>
       <c r="AS10" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT10" s="6" t="s">
         <v>54</v>
@@ -17771,7 +17774,7 @@
         <v>62</v>
       </c>
       <c r="AV10" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AW10" s="6"/>
       <c r="AX10" s="6" t="s">
@@ -17802,10 +17805,10 @@
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B11" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>43</v>
@@ -17826,7 +17829,7 @@
         <v>46</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>93</v>
@@ -17842,7 +17845,7 @@
         <v>47</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>74</v>
@@ -17863,7 +17866,7 @@
         <v>99</v>
       </c>
       <c r="V11" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W11" s="6" t="s">
         <v>100</v>
@@ -17875,10 +17878,10 @@
         <v>44</v>
       </c>
       <c r="Z11" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA11" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB11" s="6" t="s">
         <v>49</v>
@@ -17930,7 +17933,7 @@
         <v>54</v>
       </c>
       <c r="AS11" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT11" s="6" t="s">
         <v>54</v>
@@ -17939,7 +17942,7 @@
         <v>62</v>
       </c>
       <c r="AV11" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AW11" s="6"/>
       <c r="AX11" s="6" t="s">
@@ -17970,10 +17973,10 @@
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B12" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>43</v>
@@ -17994,7 +17997,7 @@
         <v>46</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>93</v>
@@ -18010,7 +18013,7 @@
         <v>47</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>75</v>
@@ -18031,7 +18034,7 @@
         <v>99</v>
       </c>
       <c r="V12" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W12" s="6" t="s">
         <v>100</v>
@@ -18043,10 +18046,10 @@
         <v>44</v>
       </c>
       <c r="Z12" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA12" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB12" s="6" t="s">
         <v>49</v>
@@ -18098,7 +18101,7 @@
         <v>54</v>
       </c>
       <c r="AS12" s="6">
-        <v>563757104</v>
+        <v>282532792</v>
       </c>
       <c r="AT12" s="6" t="s">
         <v>54</v>
@@ -18107,7 +18110,7 @@
         <v>62</v>
       </c>
       <c r="AV12" s="6" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AW12" s="6"/>
       <c r="AX12" s="6" t="s">
@@ -18138,10 +18141,10 @@
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B13" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>43</v>
@@ -18162,7 +18165,7 @@
         <v>46</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>93</v>
@@ -18178,7 +18181,7 @@
         <v>47</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>76</v>
@@ -18199,7 +18202,7 @@
         <v>99</v>
       </c>
       <c r="V13" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W13" s="6" t="s">
         <v>100</v>
@@ -18211,10 +18214,10 @@
         <v>44</v>
       </c>
       <c r="Z13" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA13" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>49</v>
@@ -18266,7 +18269,7 @@
         <v>54</v>
       </c>
       <c r="AS13" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT13" s="6" t="s">
         <v>54</v>
@@ -18275,7 +18278,7 @@
         <v>62</v>
       </c>
       <c r="AV13" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AW13" s="6"/>
       <c r="AX13" s="6" t="s">
@@ -18306,10 +18309,10 @@
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B14" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>43</v>
@@ -18330,7 +18333,7 @@
         <v>46</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>93</v>
@@ -18346,7 +18349,7 @@
         <v>47</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>77</v>
@@ -18367,7 +18370,7 @@
         <v>99</v>
       </c>
       <c r="V14" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W14" s="6" t="s">
         <v>100</v>
@@ -18379,10 +18382,10 @@
         <v>44</v>
       </c>
       <c r="Z14" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA14" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB14" s="6" t="s">
         <v>49</v>
@@ -18434,7 +18437,7 @@
         <v>54</v>
       </c>
       <c r="AS14" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT14" s="6" t="s">
         <v>54</v>
@@ -18443,7 +18446,7 @@
         <v>62</v>
       </c>
       <c r="AV14" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AW14" s="6"/>
       <c r="AX14" s="6" t="s">
@@ -18474,10 +18477,10 @@
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B15" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>43</v>
@@ -18498,7 +18501,7 @@
         <v>46</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>93</v>
@@ -18514,7 +18517,7 @@
         <v>47</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>78</v>
@@ -18535,7 +18538,7 @@
         <v>99</v>
       </c>
       <c r="V15" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W15" s="6" t="s">
         <v>100</v>
@@ -18547,10 +18550,10 @@
         <v>44</v>
       </c>
       <c r="Z15" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA15" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB15" s="6" t="s">
         <v>49</v>
@@ -18602,7 +18605,7 @@
         <v>54</v>
       </c>
       <c r="AS15" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT15" s="6" t="s">
         <v>54</v>
@@ -18611,7 +18614,7 @@
         <v>62</v>
       </c>
       <c r="AV15" s="6" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AW15" s="6"/>
       <c r="AX15" s="6" t="s">
@@ -18642,10 +18645,10 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B16" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>43</v>
@@ -18666,7 +18669,7 @@
         <v>46</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>93</v>
@@ -18682,7 +18685,7 @@
         <v>47</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>79</v>
@@ -18703,7 +18706,7 @@
         <v>99</v>
       </c>
       <c r="V16" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W16" s="6" t="s">
         <v>100</v>
@@ -18715,10 +18718,10 @@
         <v>44</v>
       </c>
       <c r="Z16" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA16" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB16" s="6" t="s">
         <v>49</v>
@@ -18770,7 +18773,7 @@
         <v>54</v>
       </c>
       <c r="AS16" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT16" s="6" t="s">
         <v>54</v>
@@ -18779,7 +18782,7 @@
         <v>62</v>
       </c>
       <c r="AV16" s="6" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AW16" s="6"/>
       <c r="AX16" s="6" t="s">
@@ -18810,10 +18813,10 @@
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B17" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>43</v>
@@ -18834,7 +18837,7 @@
         <v>46</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>93</v>
@@ -18850,7 +18853,7 @@
         <v>47</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>80</v>
@@ -18871,7 +18874,7 @@
         <v>99</v>
       </c>
       <c r="V17" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W17" s="6" t="s">
         <v>100</v>
@@ -18883,10 +18886,10 @@
         <v>44</v>
       </c>
       <c r="Z17" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA17" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB17" s="6" t="s">
         <v>49</v>
@@ -18938,7 +18941,7 @@
         <v>54</v>
       </c>
       <c r="AS17" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT17" s="6" t="s">
         <v>54</v>
@@ -18947,7 +18950,7 @@
         <v>62</v>
       </c>
       <c r="AV17" s="6" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AW17" s="6"/>
       <c r="AX17" s="6" t="s">
@@ -18978,10 +18981,10 @@
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B18" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>43</v>
@@ -19002,7 +19005,7 @@
         <v>46</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>93</v>
@@ -19018,7 +19021,7 @@
         <v>47</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>81</v>
@@ -19039,7 +19042,7 @@
         <v>99</v>
       </c>
       <c r="V18" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W18" s="6" t="s">
         <v>100</v>
@@ -19051,10 +19054,10 @@
         <v>44</v>
       </c>
       <c r="Z18" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA18" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB18" s="6" t="s">
         <v>49</v>
@@ -19106,7 +19109,7 @@
         <v>54</v>
       </c>
       <c r="AS18" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT18" s="6" t="s">
         <v>54</v>
@@ -19115,7 +19118,7 @@
         <v>62</v>
       </c>
       <c r="AV18" s="6" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AW18" s="6"/>
       <c r="AX18" s="6" t="s">
@@ -19146,10 +19149,10 @@
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B19" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>43</v>
@@ -19170,7 +19173,7 @@
         <v>46</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>93</v>
@@ -19186,7 +19189,7 @@
         <v>47</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>82</v>
@@ -19207,7 +19210,7 @@
         <v>99</v>
       </c>
       <c r="V19" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W19" s="6" t="s">
         <v>100</v>
@@ -19219,10 +19222,10 @@
         <v>44</v>
       </c>
       <c r="Z19" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA19" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB19" s="6" t="s">
         <v>49</v>
@@ -19274,7 +19277,7 @@
         <v>54</v>
       </c>
       <c r="AS19" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT19" s="6" t="s">
         <v>54</v>
@@ -19283,7 +19286,7 @@
         <v>62</v>
       </c>
       <c r="AV19" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AW19" s="6"/>
       <c r="AX19" s="6" t="s">
@@ -19314,10 +19317,10 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B20" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>43</v>
@@ -19338,7 +19341,7 @@
         <v>46</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>93</v>
@@ -19354,7 +19357,7 @@
         <v>47</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>83</v>
@@ -19375,7 +19378,7 @@
         <v>99</v>
       </c>
       <c r="V20" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W20" s="6" t="s">
         <v>100</v>
@@ -19387,10 +19390,10 @@
         <v>44</v>
       </c>
       <c r="Z20" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA20" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB20" s="6" t="s">
         <v>49</v>
@@ -19442,7 +19445,7 @@
         <v>54</v>
       </c>
       <c r="AS20" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT20" s="6" t="s">
         <v>54</v>
@@ -19451,7 +19454,7 @@
         <v>62</v>
       </c>
       <c r="AV20" s="6" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AW20" s="6"/>
       <c r="AX20" s="6" t="s">
@@ -19482,10 +19485,10 @@
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B21" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>43</v>
@@ -19506,7 +19509,7 @@
         <v>46</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>93</v>
@@ -19522,7 +19525,7 @@
         <v>47</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>84</v>
@@ -19543,7 +19546,7 @@
         <v>99</v>
       </c>
       <c r="V21" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W21" s="6" t="s">
         <v>100</v>
@@ -19555,10 +19558,10 @@
         <v>44</v>
       </c>
       <c r="Z21" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA21" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB21" s="6" t="s">
         <v>49</v>
@@ -19610,7 +19613,7 @@
         <v>54</v>
       </c>
       <c r="AS21" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT21" s="6" t="s">
         <v>54</v>
@@ -19619,7 +19622,7 @@
         <v>62</v>
       </c>
       <c r="AV21" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AW21" s="6"/>
       <c r="AX21" s="6" t="s">
@@ -19650,10 +19653,10 @@
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B22" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>43</v>
@@ -19674,7 +19677,7 @@
         <v>46</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>93</v>
@@ -19690,7 +19693,7 @@
         <v>47</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>85</v>
@@ -19711,7 +19714,7 @@
         <v>99</v>
       </c>
       <c r="V22" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W22" s="6" t="s">
         <v>100</v>
@@ -19723,10 +19726,10 @@
         <v>44</v>
       </c>
       <c r="Z22" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA22" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB22" s="6" t="s">
         <v>49</v>
@@ -19778,7 +19781,7 @@
         <v>54</v>
       </c>
       <c r="AS22" s="6">
-        <v>563757104</v>
+        <v>282446688</v>
       </c>
       <c r="AT22" s="6" t="s">
         <v>54</v>
@@ -19787,7 +19790,7 @@
         <v>62</v>
       </c>
       <c r="AV22" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AW22" s="6"/>
       <c r="AX22" s="6" t="s">
@@ -19818,10 +19821,10 @@
     </row>
     <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B23" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>43</v>
@@ -19842,7 +19845,7 @@
         <v>46</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>93</v>
@@ -19858,7 +19861,7 @@
         <v>47</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>86</v>
@@ -19879,7 +19882,7 @@
         <v>99</v>
       </c>
       <c r="V23" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W23" s="6" t="s">
         <v>100</v>
@@ -19891,10 +19894,10 @@
         <v>44</v>
       </c>
       <c r="Z23" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA23" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB23" s="6" t="s">
         <v>49</v>
@@ -19946,7 +19949,7 @@
         <v>54</v>
       </c>
       <c r="AS23" s="6">
-        <v>563757104</v>
+        <v>282354944</v>
       </c>
       <c r="AT23" s="6" t="s">
         <v>54</v>
@@ -19955,7 +19958,7 @@
         <v>62</v>
       </c>
       <c r="AV23" s="6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AW23" s="6"/>
       <c r="AX23" s="6" t="s">
@@ -19986,10 +19989,10 @@
     </row>
     <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B24" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>43</v>
@@ -20010,7 +20013,7 @@
         <v>46</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>93</v>
@@ -20026,7 +20029,7 @@
         <v>47</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>87</v>
@@ -20047,7 +20050,7 @@
         <v>99</v>
       </c>
       <c r="V24" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W24" s="6" t="s">
         <v>100</v>
@@ -20059,10 +20062,10 @@
         <v>44</v>
       </c>
       <c r="Z24" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA24" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB24" s="6" t="s">
         <v>49</v>
@@ -20114,7 +20117,7 @@
         <v>54</v>
       </c>
       <c r="AS24" s="6">
-        <v>563722512</v>
+        <v>282354944</v>
       </c>
       <c r="AT24" s="6" t="s">
         <v>54</v>
@@ -20123,7 +20126,7 @@
         <v>62</v>
       </c>
       <c r="AV24" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AW24" s="6"/>
       <c r="AX24" s="6" t="s">
@@ -20154,10 +20157,10 @@
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B25" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>43</v>
@@ -20178,7 +20181,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>93</v>
@@ -20194,7 +20197,7 @@
         <v>47</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>88</v>
@@ -20215,7 +20218,7 @@
         <v>99</v>
       </c>
       <c r="V25" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W25" s="6" t="s">
         <v>100</v>
@@ -20227,10 +20230,10 @@
         <v>44</v>
       </c>
       <c r="Z25" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA25" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB25" s="6" t="s">
         <v>49</v>
@@ -20282,7 +20285,7 @@
         <v>54</v>
       </c>
       <c r="AS25" s="6">
-        <v>563757104</v>
+        <v>282475264</v>
       </c>
       <c r="AT25" s="6" t="s">
         <v>54</v>
@@ -20291,7 +20294,7 @@
         <v>62</v>
       </c>
       <c r="AV25" s="6" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AW25" s="6"/>
       <c r="AX25" s="6" t="s">
@@ -20322,10 +20325,10 @@
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B26" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>43</v>
@@ -20346,7 +20349,7 @@
         <v>46</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>93</v>
@@ -20362,7 +20365,7 @@
         <v>47</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>89</v>
@@ -20383,7 +20386,7 @@
         <v>99</v>
       </c>
       <c r="V26" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W26" s="6" t="s">
         <v>100</v>
@@ -20395,10 +20398,10 @@
         <v>44</v>
       </c>
       <c r="Z26" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA26" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB26" s="6" t="s">
         <v>49</v>
@@ -20450,7 +20453,7 @@
         <v>54</v>
       </c>
       <c r="AS26" s="6">
-        <v>563757104</v>
+        <v>282504028</v>
       </c>
       <c r="AT26" s="6" t="s">
         <v>54</v>
@@ -20459,7 +20462,7 @@
         <v>62</v>
       </c>
       <c r="AV26" s="6" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AW26" s="6"/>
       <c r="AX26" s="6" t="s">
@@ -20490,10 +20493,10 @@
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B27" s="3">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>43</v>
@@ -20514,7 +20517,7 @@
         <v>46</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>93</v>
@@ -20530,7 +20533,7 @@
         <v>47</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>90</v>
@@ -20545,13 +20548,13 @@
         <v>64</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>98</v>
+        <v>308</v>
       </c>
       <c r="U27" s="5" t="s">
         <v>99</v>
       </c>
       <c r="V27" s="6">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="W27" s="6" t="s">
         <v>100</v>
@@ -20563,10 +20566,10 @@
         <v>44</v>
       </c>
       <c r="Z27" s="3">
-        <v>43565</v>
+        <v>44013</v>
       </c>
       <c r="AA27" s="3">
-        <v>45046</v>
+        <v>45473</v>
       </c>
       <c r="AB27" s="6" t="s">
         <v>49</v>
@@ -20618,7 +20621,7 @@
         <v>54</v>
       </c>
       <c r="AS27" s="6">
-        <v>563757104</v>
+        <v>281907316</v>
       </c>
       <c r="AT27" s="6" t="s">
         <v>54</v>
@@ -20627,7 +20630,7 @@
         <v>62</v>
       </c>
       <c r="AV27" s="6" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="AW27" s="6"/>
       <c r="AX27" s="6" t="s">
@@ -20653,7 +20656,7 @@
         <v>60</v>
       </c>
       <c r="BF27" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Serie Los cuentos de Yétili: El cascanueces SD - HD 101
</commit_message>
<xml_diff>
--- a/Run_File.xlsx
+++ b/Run_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213F5B9D-B584-44E6-A355-E16BDA417181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB7C8C-9624-4BCB-95CA-83CE95521E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1FC338CE-84E3-4770-AC7F-D0408B7F2F20}"/>
   </bookViews>
@@ -233,76 +233,76 @@
     <t>EP 01</t>
   </si>
   <si>
-    <t>EEZIBI101_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEZI6000000000000101</t>
-  </si>
-  <si>
-    <t>Serie Zibilla</t>
-  </si>
-  <si>
-    <t>ZibillaT01EP01</t>
-  </si>
-  <si>
-    <t>Zibilla T01 EP01</t>
-  </si>
-  <si>
-    <t>Edye presenta: Zibilla es diferente y sus compañeros en la escuela no la aceptan.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Zibilla es diferente y sus compañeros en la escuela no la aceptan. Tras vivir una emocionante aventura y conocer a un león salvaje, gana la confianza en sí misma necesaria para defenderse. Junto a un nuevo amigo será más fuerte.</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>00:26:10</t>
+    <t>EEYTSP101_SD_ADI.XML</t>
   </si>
   <si>
-    <t>00:26</t>
+    <t>EEYT6000000000000101</t>
   </si>
   <si>
-    <t>Infantil/Zibilla</t>
+    <t>Serie Los cuentos de Yétili: El cascanueces</t>
   </si>
   <si>
-    <t>Zibilla</t>
+    <t>Los cuentos de Yétili: El cascanuecesT01EP01</t>
   </si>
   <si>
-    <t>CH</t>
+    <t>Los cuentos de Yétili: El cascanueces T01 EP01</t>
   </si>
   <si>
-    <t>Lily Demuynck-Deydier, Arthur Ponsot, Christian Léonard, Annick Lambert</t>
+    <t>Edye presenta: Es la noche antes de Navidad. Alguien dejó un libro en el regazo de Yétili: El cascanueces.</t>
   </si>
   <si>
-    <t>Nadasdy Film Sarl</t>
+    <t>Edye presenta: Es la noche antes de Navidad. La librería cierra después de que se hayan ido los últimos clientes. Yétili puede despertar. Oh. Alguien dejó un libro en su regazo: El cascanueces. Los ratones descubrirán una historia increíble a través de la música.</t>
   </si>
   <si>
-    <t>Demuynck-Deydier Lily, Ponsot Arthur, Léonard Christian, Lambert Annick</t>
+    <t>00:26:47</t>
   </si>
   <si>
-    <t>Favez, Isabelle</t>
+    <t>00:27</t>
   </si>
   <si>
-    <t>EEZIBI101.mpg</t>
+    <t>Infantil/Los cuentos de Yétili: El cascanueces</t>
   </si>
   <si>
-    <t>EEZIBI1_box.jpg</t>
+    <t>Los cuentos de Yétili: El cascanueces</t>
   </si>
   <si>
-    <t>EEZIBI101_land.jpg</t>
+    <t>FR</t>
   </si>
   <si>
-    <t>EEZIBI101_HD_ADI.XML</t>
+    <t>Kaycie Chase, Ken Starcevic</t>
   </si>
   <si>
-    <t>EEZI7000000000000101</t>
+    <t>Puppet Moving</t>
   </si>
   <si>
-    <t>Zibilla T01 EP01 HD</t>
+    <t>Chase Kaycie, Starcevic Ken</t>
   </si>
   <si>
-    <t>EEZIBI101.ts</t>
+    <t>Montagnese, Emeric</t>
+  </si>
+  <si>
+    <t>EEYTSP101.mpg</t>
+  </si>
+  <si>
+    <t>EEYTSP1_box.jpg</t>
+  </si>
+  <si>
+    <t>EEYTSP101_land.jpg</t>
+  </si>
+  <si>
+    <t>EEYTSP101_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEYT7000000000000101</t>
+  </si>
+  <si>
+    <t>Los cuentos de Yétili: El cascanueces T01 EP01 HD</t>
+  </si>
+  <si>
+    <t>EEYTSP101.ts</t>
   </si>
 </sst>
 </file>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3">
         <v>44628</v>
@@ -6816,13 +6816,13 @@
         <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -6832,19 +6832,19 @@
         <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>64</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>73</v>
@@ -6853,7 +6853,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -6865,10 +6865,10 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>44532</v>
+        <v>44561</v>
       </c>
       <c r="AA2" s="3">
-        <v>45260</v>
+        <v>45290</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>49</v>
@@ -6920,7 +6920,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>736648484</v>
+        <v>754061796</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>55</v>
@@ -12642,10 +12642,10 @@
         <v>86</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
@@ -12661,13 +12661,13 @@
         <v>64</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>73</v>
@@ -12676,7 +12676,7 @@
         <v>74</v>
       </c>
       <c r="V2" s="6">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>75</v>
@@ -12688,10 +12688,10 @@
         <v>44</v>
       </c>
       <c r="Z2" s="3">
-        <v>44532</v>
+        <v>44561</v>
       </c>
       <c r="AA2" s="3">
-        <v>45260</v>
+        <v>45290</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>49</v>
@@ -12743,7 +12743,7 @@
         <v>54</v>
       </c>
       <c r="AS2" s="6">
-        <v>1473233424</v>
+        <v>1508065876</v>
       </c>
       <c r="AT2" s="6" t="s">
         <v>54</v>

</xml_diff>